<commit_message>
Se agrega la variable tipo banco para valida los datos donde son destinados, Banacolombia o Davivienda
</commit_message>
<xml_diff>
--- a/reporte de cuentas por pagar.xlsx
+++ b/reporte de cuentas por pagar.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\Diana\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Diana\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE958B3E-A588-4419-9665-F282FC083CD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486353E0-DDDA-4A30-9B7E-2924A48D59E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1815" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExportarAExcel" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="317">
   <si>
     <t>Nombres</t>
   </si>
@@ -186,9 +186,6 @@
     <t>CIMPRE SALUD OCUPACIONAL S.A.S.</t>
   </si>
   <si>
-    <t>NIT 800033294 - 2</t>
-  </si>
-  <si>
     <t>393</t>
   </si>
   <si>
@@ -540,9 +537,6 @@
     <t>IZC MAYORISTA SAS</t>
   </si>
   <si>
-    <t>NIT 800153963 - 6</t>
-  </si>
-  <si>
     <t>10189</t>
   </si>
   <si>
@@ -982,6 +976,18 @@
   </si>
   <si>
     <t>Total JOHN JAIRO BUENO SALAZAR</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>NIT 1143940722 - 6</t>
+  </si>
+  <si>
+    <t>NIT 1143940723 - 2</t>
   </si>
 </sst>
 </file>
@@ -1526,10 +1532,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Hoja1"/>
+  <sheetPr codeName="Hoja1" filterMode="1"/>
   <dimension ref="A1:P214"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I204" sqref="I204"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="4" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1547,7 +1555,8 @@
     <col min="12" max="12" width="14.28515625" style="4" customWidth="1"/>
     <col min="13" max="13" width="21.42578125" style="22" customWidth="1"/>
     <col min="14" max="14" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="2"/>
+    <col min="15" max="15" width="25.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
@@ -1598,7 +1607,7 @@
       </c>
       <c r="P1" s="22"/>
     </row>
-    <row r="2" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
         <v>15</v>
       </c>
@@ -1639,7 +1648,7 @@
       <c r="O2" s="22"/>
       <c r="P2" s="22"/>
     </row>
-    <row r="3" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
         <v>19</v>
       </c>
@@ -1680,7 +1689,7 @@
       <c r="O3" s="22"/>
       <c r="P3" s="22"/>
     </row>
-    <row r="4" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
         <v>19</v>
       </c>
@@ -1721,7 +1730,7 @@
       <c r="O4" s="22"/>
       <c r="P4" s="22"/>
     </row>
-    <row r="5" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A5" s="22"/>
       <c r="B5" s="23"/>
       <c r="C5" s="24"/>
@@ -1750,7 +1759,7 @@
       <c r="O5" s="22"/>
       <c r="P5" s="22"/>
     </row>
-    <row r="6" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>22</v>
       </c>
@@ -1783,7 +1792,7 @@
       <c r="O6" s="22"/>
       <c r="P6" s="22"/>
     </row>
-    <row r="7" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
         <v>23</v>
       </c>
@@ -1824,7 +1833,7 @@
       <c r="O7" s="22"/>
       <c r="P7" s="22"/>
     </row>
-    <row r="8" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
         <v>19</v>
       </c>
@@ -1865,7 +1874,7 @@
       <c r="O8" s="22"/>
       <c r="P8" s="22"/>
     </row>
-    <row r="9" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24"/>
@@ -1894,7 +1903,7 @@
       <c r="O9" s="22"/>
       <c r="P9" s="22"/>
     </row>
-    <row r="10" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
         <v>27</v>
       </c>
@@ -1927,7 +1936,7 @@
       <c r="O10" s="22"/>
       <c r="P10" s="22"/>
     </row>
-    <row r="11" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A11" s="22" t="s">
         <v>28</v>
       </c>
@@ -1968,7 +1977,7 @@
       <c r="O11" s="22"/>
       <c r="P11" s="22"/>
     </row>
-    <row r="12" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A12" s="22" t="s">
         <v>19</v>
       </c>
@@ -2009,7 +2018,7 @@
       <c r="O12" s="22"/>
       <c r="P12" s="22"/>
     </row>
-    <row r="13" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A13" s="22" t="s">
         <v>19</v>
       </c>
@@ -2050,7 +2059,7 @@
       <c r="O13" s="22"/>
       <c r="P13" s="22"/>
     </row>
-    <row r="14" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A14" s="22"/>
       <c r="B14" s="23"/>
       <c r="C14" s="24"/>
@@ -2079,7 +2088,7 @@
       <c r="O14" s="22"/>
       <c r="P14" s="22"/>
     </row>
-    <row r="15" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="s">
         <v>33</v>
       </c>
@@ -2160,10 +2169,12 @@
         <f>H11+H12+H13</f>
         <v>2359386</v>
       </c>
-      <c r="O16" s="27"/>
+      <c r="O16" s="27" t="s">
+        <v>314</v>
+      </c>
       <c r="P16" s="27"/>
     </row>
-    <row r="17" spans="1:16" s="6" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" s="6" customFormat="1" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A17" s="27" t="s">
         <v>19</v>
       </c>
@@ -2207,7 +2218,7 @@
       <c r="O17" s="27"/>
       <c r="P17" s="27"/>
     </row>
-    <row r="18" spans="1:16" s="6" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" s="6" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A18" s="27"/>
       <c r="B18" s="7"/>
       <c r="C18" s="20"/>
@@ -2237,7 +2248,7 @@
       <c r="O18" s="27"/>
       <c r="P18" s="27"/>
     </row>
-    <row r="19" spans="1:16" s="6" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" s="6" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
         <v>41</v>
       </c>
@@ -2316,10 +2327,12 @@
         <f>H16+H17</f>
         <v>525870</v>
       </c>
-      <c r="O20" s="22"/>
+      <c r="O20" s="27" t="s">
+        <v>314</v>
+      </c>
       <c r="P20" s="22"/>
     </row>
-    <row r="21" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A21" s="22"/>
       <c r="B21" s="23"/>
       <c r="C21" s="24"/>
@@ -2348,7 +2361,7 @@
       <c r="O21" s="22"/>
       <c r="P21" s="22"/>
     </row>
-    <row r="22" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A22" s="25" t="s">
         <v>46</v>
       </c>
@@ -2390,13 +2403,13 @@
         <v>48</v>
       </c>
       <c r="B23" s="23" t="s">
+        <v>316</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="24" t="s">
         <v>49</v>
-      </c>
-      <c r="C23" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="24" t="s">
-        <v>50</v>
       </c>
       <c r="E23" s="17">
         <v>44105</v>
@@ -2423,16 +2436,18 @@
         <v>0</v>
       </c>
       <c r="M23" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N23" s="24">
         <f>J20</f>
         <v>87451</v>
       </c>
-      <c r="O23" s="22"/>
+      <c r="O23" s="27" t="s">
+        <v>314</v>
+      </c>
       <c r="P23" s="22"/>
     </row>
-    <row r="24" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A24" s="22"/>
       <c r="B24" s="23"/>
       <c r="C24" s="24"/>
@@ -2461,9 +2476,9 @@
       <c r="O24" s="22"/>
       <c r="P24" s="22"/>
     </row>
-    <row r="25" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A25" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B25" s="23" t="s">
         <v>19</v>
@@ -2495,21 +2510,21 @@
         <v>84300</v>
       </c>
       <c r="P25" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="6" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A26" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="C26" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="20" t="s">
         <v>55</v>
-      </c>
-      <c r="C26" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="D26" s="20" t="s">
-        <v>56</v>
       </c>
       <c r="E26" s="8">
         <v>44105</v>
@@ -2540,10 +2555,12 @@
         <f>H23</f>
         <v>84300</v>
       </c>
-      <c r="O26" s="27"/>
+      <c r="O26" s="27" t="s">
+        <v>314</v>
+      </c>
       <c r="P26" s="27"/>
     </row>
-    <row r="27" spans="1:16" s="6" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" s="6" customFormat="1" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A27" s="27" t="s">
         <v>19</v>
       </c>
@@ -2554,7 +2571,7 @@
         <v>17</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E27" s="8">
         <v>44105</v>
@@ -2585,7 +2602,7 @@
       <c r="O27" s="27"/>
       <c r="P27" s="27"/>
     </row>
-    <row r="28" spans="1:16" s="6" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" s="6" customFormat="1" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A28" s="27" t="s">
         <v>19</v>
       </c>
@@ -2596,7 +2613,7 @@
         <v>17</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E28" s="8">
         <v>44105</v>
@@ -2627,7 +2644,7 @@
       <c r="O28" s="27"/>
       <c r="P28" s="27"/>
     </row>
-    <row r="29" spans="1:16" s="6" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" s="6" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A29" s="27"/>
       <c r="B29" s="7"/>
       <c r="C29" s="20"/>
@@ -2657,9 +2674,9 @@
       <c r="O29" s="27"/>
       <c r="P29" s="27"/>
     </row>
-    <row r="30" spans="1:16" s="6" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" s="6" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>19</v>
@@ -2693,16 +2710,16 @@
     </row>
     <row r="31" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A31" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="23" t="s">
+      <c r="C31" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="24" t="s">
         <v>61</v>
-      </c>
-      <c r="C31" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D31" s="24" t="s">
-        <v>62</v>
       </c>
       <c r="E31" s="17">
         <v>44117</v>
@@ -2732,10 +2749,12 @@
         <f>I26+I27+I28</f>
         <v>193970</v>
       </c>
-      <c r="O31" s="22"/>
+      <c r="O31" s="27" t="s">
+        <v>314</v>
+      </c>
       <c r="P31" s="22"/>
     </row>
-    <row r="32" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A32" s="22" t="s">
         <v>19</v>
       </c>
@@ -2746,7 +2765,7 @@
         <v>17</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E32" s="17">
         <v>44119</v>
@@ -2776,7 +2795,7 @@
       <c r="O32" s="22"/>
       <c r="P32" s="22"/>
     </row>
-    <row r="33" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A33" s="22"/>
       <c r="B33" s="23"/>
       <c r="C33" s="24"/>
@@ -2805,9 +2824,9 @@
       <c r="O33" s="22"/>
       <c r="P33" s="22"/>
     </row>
-    <row r="34" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A34" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B34" s="23" t="s">
         <v>19</v>
@@ -2838,18 +2857,18 @@
       <c r="O34" s="22"/>
       <c r="P34" s="22"/>
     </row>
-    <row r="35" spans="1:16" s="6" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" s="6" customFormat="1" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A35" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="C35" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="20" t="s">
         <v>66</v>
-      </c>
-      <c r="C35" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="D35" s="20" t="s">
-        <v>67</v>
       </c>
       <c r="E35" s="8">
         <v>44119</v>
@@ -2880,7 +2899,7 @@
       <c r="O35" s="27"/>
       <c r="P35" s="27"/>
     </row>
-    <row r="36" spans="1:16" s="6" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" s="6" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A36" s="27"/>
       <c r="B36" s="7"/>
       <c r="C36" s="20"/>
@@ -2910,9 +2929,9 @@
       <c r="O36" s="27"/>
       <c r="P36" s="27"/>
     </row>
-    <row r="37" spans="1:16" s="6" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" s="6" customFormat="1" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>19</v>
@@ -2945,21 +2964,21 @@
         <v>97991</v>
       </c>
       <c r="P37" s="27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A38" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="B38" s="23" t="s">
+      <c r="C38" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="24" t="s">
         <v>71</v>
-      </c>
-      <c r="C38" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D38" s="24" t="s">
-        <v>72</v>
       </c>
       <c r="E38" s="17">
         <v>44106</v>
@@ -2986,16 +3005,18 @@
         <v>0</v>
       </c>
       <c r="M38" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N38" s="24">
         <f>H35</f>
         <v>97991</v>
       </c>
-      <c r="O38" s="22"/>
+      <c r="O38" s="27" t="s">
+        <v>313</v>
+      </c>
       <c r="P38" s="22"/>
     </row>
-    <row r="39" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A39" s="22"/>
       <c r="B39" s="23"/>
       <c r="C39" s="24"/>
@@ -3024,9 +3045,9 @@
       <c r="O39" s="22"/>
       <c r="P39" s="22"/>
     </row>
-    <row r="40" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A40" s="25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B40" s="23" t="s">
         <v>19</v>
@@ -3054,24 +3075,24 @@
         <v>0</v>
       </c>
       <c r="M40" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N40" s="22"/>
       <c r="O40" s="22"/>
       <c r="P40" s="22"/>
     </row>
-    <row r="41" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A41" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="B41" s="23" t="s">
+      <c r="C41" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" s="24" t="s">
         <v>77</v>
-      </c>
-      <c r="C41" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D41" s="24" t="s">
-        <v>78</v>
       </c>
       <c r="E41" s="17">
         <v>44089</v>
@@ -3101,7 +3122,7 @@
       <c r="O41" s="22"/>
       <c r="P41" s="22"/>
     </row>
-    <row r="42" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A42" s="22"/>
       <c r="B42" s="23"/>
       <c r="C42" s="24"/>
@@ -3130,9 +3151,9 @@
       <c r="O42" s="22"/>
       <c r="P42" s="22"/>
     </row>
-    <row r="43" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A43" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B43" s="23" t="s">
         <v>19</v>
@@ -3167,16 +3188,16 @@
     </row>
     <row r="44" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A44" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="B44" s="23" t="s">
+      <c r="C44" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="24" t="s">
         <v>81</v>
-      </c>
-      <c r="C44" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D44" s="24" t="s">
-        <v>82</v>
       </c>
       <c r="E44" s="17">
         <v>44106</v>
@@ -3206,10 +3227,12 @@
         <f>I41</f>
         <v>172500</v>
       </c>
-      <c r="O44" s="22"/>
+      <c r="O44" s="27" t="s">
+        <v>314</v>
+      </c>
       <c r="P44" s="22"/>
     </row>
-    <row r="45" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A45" s="22" t="s">
         <v>19</v>
       </c>
@@ -3220,7 +3243,7 @@
         <v>17</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E45" s="17">
         <v>44106</v>
@@ -3250,7 +3273,7 @@
       <c r="O45" s="22"/>
       <c r="P45" s="22"/>
     </row>
-    <row r="46" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A46" s="22" t="s">
         <v>19</v>
       </c>
@@ -3261,7 +3284,7 @@
         <v>17</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E46" s="17">
         <v>44118</v>
@@ -3291,7 +3314,7 @@
       <c r="O46" s="22"/>
       <c r="P46" s="22"/>
     </row>
-    <row r="47" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A47" s="22" t="s">
         <v>19</v>
       </c>
@@ -3302,7 +3325,7 @@
         <v>17</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E47" s="17">
         <v>44098</v>
@@ -3332,7 +3355,7 @@
       <c r="O47" s="22"/>
       <c r="P47" s="22"/>
     </row>
-    <row r="48" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A48" s="22" t="s">
         <v>19</v>
       </c>
@@ -3343,7 +3366,7 @@
         <v>17</v>
       </c>
       <c r="D48" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E48" s="17">
         <v>44098</v>
@@ -3373,7 +3396,7 @@
       <c r="O48" s="22"/>
       <c r="P48" s="22"/>
     </row>
-    <row r="49" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A49" s="22"/>
       <c r="B49" s="23"/>
       <c r="C49" s="24"/>
@@ -3402,9 +3425,9 @@
       <c r="O49" s="22"/>
       <c r="P49" s="22"/>
     </row>
-    <row r="50" spans="1:16" ht="12" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" ht="12" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A50" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B50" s="23" t="s">
         <v>19</v>
@@ -3436,21 +3459,21 @@
         <v>1819546</v>
       </c>
       <c r="P50" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51" spans="1:16" s="13" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A51" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B51" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="C51" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D51" s="20" t="s">
         <v>90</v>
-      </c>
-      <c r="C51" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="D51" s="20" t="s">
-        <v>91</v>
       </c>
       <c r="E51" s="8">
         <v>44105</v>
@@ -3481,10 +3504,12 @@
         <f>H47+H48</f>
         <v>1819546</v>
       </c>
-      <c r="O51" s="27"/>
+      <c r="O51" s="27" t="s">
+        <v>314</v>
+      </c>
       <c r="P51" s="27"/>
     </row>
-    <row r="52" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A52" s="22" t="s">
         <v>19</v>
       </c>
@@ -3495,7 +3520,7 @@
         <v>17</v>
       </c>
       <c r="D52" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E52" s="17">
         <v>44083</v>
@@ -3525,7 +3550,7 @@
       <c r="O52" s="22"/>
       <c r="P52" s="22"/>
     </row>
-    <row r="53" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A53" s="22" t="s">
         <v>19</v>
       </c>
@@ -3536,7 +3561,7 @@
         <v>17</v>
       </c>
       <c r="D53" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E53" s="17">
         <v>44055</v>
@@ -3566,7 +3591,7 @@
       <c r="O53" s="22"/>
       <c r="P53" s="22"/>
     </row>
-    <row r="54" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A54" s="22" t="s">
         <v>19</v>
       </c>
@@ -3577,7 +3602,7 @@
         <v>17</v>
       </c>
       <c r="D54" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E54" s="17">
         <v>44113</v>
@@ -3607,7 +3632,7 @@
       <c r="O54" s="22"/>
       <c r="P54" s="22"/>
     </row>
-    <row r="55" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A55" s="22" t="s">
         <v>19</v>
       </c>
@@ -3618,7 +3643,7 @@
         <v>17</v>
       </c>
       <c r="D55" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E55" s="17">
         <v>44081</v>
@@ -3648,7 +3673,7 @@
       <c r="O55" s="22"/>
       <c r="P55" s="22"/>
     </row>
-    <row r="56" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A56" s="22" t="s">
         <v>19</v>
       </c>
@@ -3659,7 +3684,7 @@
         <v>17</v>
       </c>
       <c r="D56" s="24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E56" s="17">
         <v>44076</v>
@@ -3689,7 +3714,7 @@
       <c r="O56" s="22"/>
       <c r="P56" s="22"/>
     </row>
-    <row r="57" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A57" s="22" t="s">
         <v>19</v>
       </c>
@@ -3700,7 +3725,7 @@
         <v>17</v>
       </c>
       <c r="D57" s="24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E57" s="17">
         <v>44114</v>
@@ -3730,7 +3755,7 @@
       <c r="O57" s="22"/>
       <c r="P57" s="22"/>
     </row>
-    <row r="58" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A58" s="22" t="s">
         <v>19</v>
       </c>
@@ -3741,7 +3766,7 @@
         <v>17</v>
       </c>
       <c r="D58" s="24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E58" s="17">
         <v>44111</v>
@@ -3771,7 +3796,7 @@
       <c r="O58" s="22"/>
       <c r="P58" s="22"/>
     </row>
-    <row r="59" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A59" s="22" t="s">
         <v>19</v>
       </c>
@@ -3782,7 +3807,7 @@
         <v>17</v>
       </c>
       <c r="D59" s="24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E59" s="17">
         <v>44077</v>
@@ -3812,7 +3837,7 @@
       <c r="O59" s="22"/>
       <c r="P59" s="22"/>
     </row>
-    <row r="60" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A60" s="22" t="s">
         <v>19</v>
       </c>
@@ -3823,7 +3848,7 @@
         <v>17</v>
       </c>
       <c r="D60" s="24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E60" s="17">
         <v>44088</v>
@@ -3853,7 +3878,7 @@
       <c r="O60" s="22"/>
       <c r="P60" s="22"/>
     </row>
-    <row r="61" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A61" s="22" t="s">
         <v>19</v>
       </c>
@@ -3864,7 +3889,7 @@
         <v>17</v>
       </c>
       <c r="D61" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E61" s="17">
         <v>44103</v>
@@ -3894,7 +3919,7 @@
       <c r="O61" s="22"/>
       <c r="P61" s="22"/>
     </row>
-    <row r="62" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A62" s="22" t="s">
         <v>19</v>
       </c>
@@ -3905,7 +3930,7 @@
         <v>17</v>
       </c>
       <c r="D62" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E62" s="17">
         <v>44102</v>
@@ -3935,7 +3960,7 @@
       <c r="O62" s="22"/>
       <c r="P62" s="22"/>
     </row>
-    <row r="63" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A63" s="22" t="s">
         <v>19</v>
       </c>
@@ -3946,7 +3971,7 @@
         <v>17</v>
       </c>
       <c r="D63" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E63" s="17">
         <v>44074</v>
@@ -3976,7 +4001,7 @@
       <c r="O63" s="22"/>
       <c r="P63" s="22"/>
     </row>
-    <row r="64" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A64" s="22" t="s">
         <v>19</v>
       </c>
@@ -3987,7 +4012,7 @@
         <v>17</v>
       </c>
       <c r="D64" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E64" s="17">
         <v>44090</v>
@@ -4017,7 +4042,7 @@
       <c r="O64" s="22"/>
       <c r="P64" s="22"/>
     </row>
-    <row r="65" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A65" s="22" t="s">
         <v>19</v>
       </c>
@@ -4028,7 +4053,7 @@
         <v>17</v>
       </c>
       <c r="D65" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E65" s="17">
         <v>44098</v>
@@ -4058,7 +4083,7 @@
       <c r="O65" s="22"/>
       <c r="P65" s="22"/>
     </row>
-    <row r="66" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A66" s="22" t="s">
         <v>19</v>
       </c>
@@ -4069,7 +4094,7 @@
         <v>17</v>
       </c>
       <c r="D66" s="24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E66" s="17">
         <v>44099</v>
@@ -4099,7 +4124,7 @@
       <c r="O66" s="22"/>
       <c r="P66" s="22"/>
     </row>
-    <row r="67" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A67" s="22" t="s">
         <v>19</v>
       </c>
@@ -4110,7 +4135,7 @@
         <v>17</v>
       </c>
       <c r="D67" s="24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E67" s="17">
         <v>44098</v>
@@ -4140,7 +4165,7 @@
       <c r="O67" s="22"/>
       <c r="P67" s="22"/>
     </row>
-    <row r="68" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A68" s="22" t="s">
         <v>19</v>
       </c>
@@ -4151,7 +4176,7 @@
         <v>17</v>
       </c>
       <c r="D68" s="24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E68" s="17">
         <v>44071</v>
@@ -4181,7 +4206,7 @@
       <c r="O68" s="22"/>
       <c r="P68" s="22"/>
     </row>
-    <row r="69" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A69" s="22" t="s">
         <v>19</v>
       </c>
@@ -4192,7 +4217,7 @@
         <v>17</v>
       </c>
       <c r="D69" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E69" s="17">
         <v>44104</v>
@@ -4222,7 +4247,7 @@
       <c r="O69" s="22"/>
       <c r="P69" s="22"/>
     </row>
-    <row r="70" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A70" s="22"/>
       <c r="B70" s="23"/>
       <c r="C70" s="24"/>
@@ -4252,9 +4277,9 @@
       <c r="O70" s="22"/>
       <c r="P70" s="22"/>
     </row>
-    <row r="71" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A71" s="25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B71" s="23" t="s">
         <v>19</v>
@@ -4286,21 +4311,21 @@
         <v>9952604</v>
       </c>
       <c r="P71" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="72" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A72" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="B72" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="B72" s="23" t="s">
+      <c r="C72" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D72" s="24" t="s">
         <v>113</v>
-      </c>
-      <c r="C72" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D72" s="24" t="s">
-        <v>114</v>
       </c>
       <c r="E72" s="17">
         <v>44110</v>
@@ -4330,10 +4355,12 @@
         <f>I53+H68+H69</f>
         <v>9952604</v>
       </c>
-      <c r="O72" s="22"/>
+      <c r="O72" s="27" t="s">
+        <v>314</v>
+      </c>
       <c r="P72" s="22"/>
     </row>
-    <row r="73" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A73" s="22" t="s">
         <v>19</v>
       </c>
@@ -4344,7 +4371,7 @@
         <v>17</v>
       </c>
       <c r="D73" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E73" s="17">
         <v>44118</v>
@@ -4374,7 +4401,7 @@
       <c r="O73" s="22"/>
       <c r="P73" s="22"/>
     </row>
-    <row r="74" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A74" s="22" t="s">
         <v>19</v>
       </c>
@@ -4385,7 +4412,7 @@
         <v>17</v>
       </c>
       <c r="D74" s="24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E74" s="17">
         <v>44109</v>
@@ -4415,7 +4442,7 @@
       <c r="O74" s="22"/>
       <c r="P74" s="22"/>
     </row>
-    <row r="75" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A75" s="22" t="s">
         <v>19</v>
       </c>
@@ -4426,7 +4453,7 @@
         <v>17</v>
       </c>
       <c r="D75" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E75" s="17">
         <v>44088</v>
@@ -4456,7 +4483,7 @@
       <c r="O75" s="22"/>
       <c r="P75" s="22"/>
     </row>
-    <row r="76" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A76" s="22" t="s">
         <v>19</v>
       </c>
@@ -4467,7 +4494,7 @@
         <v>17</v>
       </c>
       <c r="D76" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E76" s="17">
         <v>44091</v>
@@ -4497,7 +4524,7 @@
       <c r="O76" s="22"/>
       <c r="P76" s="22"/>
     </row>
-    <row r="77" spans="1:16" ht="38.25" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16" ht="38.25" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A77" s="22" t="s">
         <v>19</v>
       </c>
@@ -4508,7 +4535,7 @@
         <v>17</v>
       </c>
       <c r="D77" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E77" s="17">
         <v>44075</v>
@@ -4535,13 +4562,13 @@
         <v>0</v>
       </c>
       <c r="M77" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N77" s="22"/>
       <c r="O77" s="22"/>
       <c r="P77" s="22"/>
     </row>
-    <row r="78" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A78" s="22" t="s">
         <v>19</v>
       </c>
@@ -4552,7 +4579,7 @@
         <v>17</v>
       </c>
       <c r="D78" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E78" s="17">
         <v>44097</v>
@@ -4582,7 +4609,7 @@
       <c r="O78" s="22"/>
       <c r="P78" s="22"/>
     </row>
-    <row r="79" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A79" s="22" t="s">
         <v>19</v>
       </c>
@@ -4593,7 +4620,7 @@
         <v>17</v>
       </c>
       <c r="D79" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E79" s="17">
         <v>44099</v>
@@ -4623,7 +4650,7 @@
       <c r="O79" s="22"/>
       <c r="P79" s="22"/>
     </row>
-    <row r="80" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A80" s="22" t="s">
         <v>19</v>
       </c>
@@ -4634,7 +4661,7 @@
         <v>17</v>
       </c>
       <c r="D80" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E80" s="17">
         <v>44104</v>
@@ -4664,7 +4691,7 @@
       <c r="O80" s="22"/>
       <c r="P80" s="22"/>
     </row>
-    <row r="81" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A81" s="22" t="s">
         <v>19</v>
       </c>
@@ -4675,7 +4702,7 @@
         <v>17</v>
       </c>
       <c r="D81" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E81" s="17">
         <v>44103</v>
@@ -4705,7 +4732,7 @@
       <c r="O81" s="22"/>
       <c r="P81" s="22"/>
     </row>
-    <row r="82" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A82" s="22" t="s">
         <v>19</v>
       </c>
@@ -4716,7 +4743,7 @@
         <v>17</v>
       </c>
       <c r="D82" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E82" s="17">
         <v>44088</v>
@@ -4743,13 +4770,13 @@
         <v>0</v>
       </c>
       <c r="M82" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N82" s="22"/>
       <c r="O82" s="22"/>
       <c r="P82" s="22"/>
     </row>
-    <row r="83" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A83" s="22"/>
       <c r="B83" s="23"/>
       <c r="C83" s="24"/>
@@ -4778,9 +4805,9 @@
       <c r="O83" s="22"/>
       <c r="P83" s="22"/>
     </row>
-    <row r="84" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A84" s="25" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B84" s="23" t="s">
         <v>19</v>
@@ -4812,21 +4839,21 @@
         <v>4407849</v>
       </c>
       <c r="P84" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="85" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A85" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="B85" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="B85" s="23" t="s">
+      <c r="C85" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D85" s="24" t="s">
         <v>130</v>
-      </c>
-      <c r="C85" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D85" s="24" t="s">
-        <v>131</v>
       </c>
       <c r="E85" s="17">
         <v>44106</v>
@@ -4856,10 +4883,12 @@
         <f>I75+H76+H78+H79</f>
         <v>4407849</v>
       </c>
-      <c r="O85" s="22"/>
+      <c r="O85" s="27" t="s">
+        <v>313</v>
+      </c>
       <c r="P85" s="22"/>
     </row>
-    <row r="86" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A86" s="22" t="s">
         <v>19</v>
       </c>
@@ -4870,7 +4899,7 @@
         <v>17</v>
       </c>
       <c r="D86" s="24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E86" s="17">
         <v>44106</v>
@@ -4900,7 +4929,7 @@
       <c r="O86" s="22"/>
       <c r="P86" s="22"/>
     </row>
-    <row r="87" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A87" s="22" t="s">
         <v>19</v>
       </c>
@@ -4911,7 +4940,7 @@
         <v>17</v>
       </c>
       <c r="D87" s="24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E87" s="17">
         <v>44106</v>
@@ -4941,7 +4970,7 @@
       <c r="O87" s="22"/>
       <c r="P87" s="22"/>
     </row>
-    <row r="88" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A88" s="22" t="s">
         <v>19</v>
       </c>
@@ -4952,7 +4981,7 @@
         <v>17</v>
       </c>
       <c r="D88" s="24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E88" s="17">
         <v>44106</v>
@@ -4982,7 +5011,7 @@
       <c r="O88" s="22"/>
       <c r="P88" s="22"/>
     </row>
-    <row r="89" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A89" s="22"/>
       <c r="B89" s="23"/>
       <c r="C89" s="24"/>
@@ -5011,9 +5040,9 @@
       <c r="O89" s="22"/>
       <c r="P89" s="22"/>
     </row>
-    <row r="90" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A90" s="25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B90" s="23" t="s">
         <v>19</v>
@@ -5044,18 +5073,18 @@
       <c r="O90" s="22"/>
       <c r="P90" s="22"/>
     </row>
-    <row r="91" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A91" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="B91" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="B91" s="23" t="s">
+      <c r="C91" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D91" s="24" t="s">
         <v>137</v>
-      </c>
-      <c r="C91" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D91" s="24" t="s">
-        <v>138</v>
       </c>
       <c r="E91" s="17">
         <v>44105</v>
@@ -5085,7 +5114,7 @@
       <c r="O91" s="22"/>
       <c r="P91" s="22"/>
     </row>
-    <row r="92" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A92" s="22"/>
       <c r="B92" s="23"/>
       <c r="C92" s="24"/>
@@ -5114,9 +5143,9 @@
       <c r="O92" s="22"/>
       <c r="P92" s="22"/>
     </row>
-    <row r="93" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A93" s="25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B93" s="23" t="s">
         <v>19</v>
@@ -5147,18 +5176,18 @@
       <c r="O93" s="22"/>
       <c r="P93" s="22"/>
     </row>
-    <row r="94" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A94" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="B94" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="B94" s="23" t="s">
+      <c r="C94" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D94" s="24" t="s">
         <v>141</v>
-      </c>
-      <c r="C94" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D94" s="24" t="s">
-        <v>142</v>
       </c>
       <c r="E94" s="17">
         <v>44112</v>
@@ -5188,7 +5217,7 @@
       <c r="O94" s="22"/>
       <c r="P94" s="22"/>
     </row>
-    <row r="95" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A95" s="22" t="s">
         <v>19</v>
       </c>
@@ -5199,7 +5228,7 @@
         <v>17</v>
       </c>
       <c r="D95" s="24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E95" s="17">
         <v>44106</v>
@@ -5229,7 +5258,7 @@
       <c r="O95" s="22"/>
       <c r="P95" s="22"/>
     </row>
-    <row r="96" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A96" s="22" t="s">
         <v>19</v>
       </c>
@@ -5240,7 +5269,7 @@
         <v>17</v>
       </c>
       <c r="D96" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E96" s="17">
         <v>44082</v>
@@ -5270,7 +5299,7 @@
       <c r="O96" s="22"/>
       <c r="P96" s="22"/>
     </row>
-    <row r="97" spans="1:12" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:12" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A97" s="22" t="s">
         <v>19</v>
       </c>
@@ -5281,7 +5310,7 @@
         <v>17</v>
       </c>
       <c r="D97" s="24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E97" s="17">
         <v>44106</v>
@@ -5308,7 +5337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:12" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:12" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A98" s="22" t="s">
         <v>19</v>
       </c>
@@ -5319,7 +5348,7 @@
         <v>17</v>
       </c>
       <c r="D98" s="24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E98" s="17">
         <v>44082</v>
@@ -5346,7 +5375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:12" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:12" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A99" s="22" t="s">
         <v>19</v>
       </c>
@@ -5357,7 +5386,7 @@
         <v>17</v>
       </c>
       <c r="D99" s="24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E99" s="17">
         <v>44110</v>
@@ -5384,7 +5413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:12" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:12" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A100" s="22" t="s">
         <v>19</v>
       </c>
@@ -5395,7 +5424,7 @@
         <v>17</v>
       </c>
       <c r="D100" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E100" s="17">
         <v>44082</v>
@@ -5422,7 +5451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:12" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:12" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A101" s="22" t="s">
         <v>19</v>
       </c>
@@ -5433,7 +5462,7 @@
         <v>17</v>
       </c>
       <c r="D101" s="24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E101" s="17">
         <v>44083</v>
@@ -5460,7 +5489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:12" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:12" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A102" s="22" t="s">
         <v>19</v>
       </c>
@@ -5471,7 +5500,7 @@
         <v>17</v>
       </c>
       <c r="D102" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E102" s="17">
         <v>44076</v>
@@ -5498,7 +5527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:12" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:12" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A103" s="22" t="s">
         <v>19</v>
       </c>
@@ -5509,7 +5538,7 @@
         <v>17</v>
       </c>
       <c r="D103" s="24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E103" s="17">
         <v>44091</v>
@@ -5536,7 +5565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:12" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:12" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A104" s="22" t="s">
         <v>19</v>
       </c>
@@ -5547,7 +5576,7 @@
         <v>17</v>
       </c>
       <c r="D104" s="24" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E104" s="17">
         <v>44089</v>
@@ -5574,7 +5603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:12" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:12" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A105" s="22" t="s">
         <v>19</v>
       </c>
@@ -5585,7 +5614,7 @@
         <v>17</v>
       </c>
       <c r="D105" s="24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E105" s="17">
         <v>44089</v>
@@ -5612,7 +5641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:12" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:12" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A106" s="22" t="s">
         <v>19</v>
       </c>
@@ -5623,7 +5652,7 @@
         <v>17</v>
       </c>
       <c r="D106" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E106" s="17">
         <v>44091</v>
@@ -5650,7 +5679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:12" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:12" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A107" s="22" t="s">
         <v>19</v>
       </c>
@@ -5661,7 +5690,7 @@
         <v>17</v>
       </c>
       <c r="D107" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E107" s="17">
         <v>44096</v>
@@ -5688,7 +5717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:12" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:12" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A108" s="22" t="s">
         <v>19</v>
       </c>
@@ -5699,7 +5728,7 @@
         <v>17</v>
       </c>
       <c r="D108" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E108" s="17">
         <v>44096</v>
@@ -5726,7 +5755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:12" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:12" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A109" s="22" t="s">
         <v>19</v>
       </c>
@@ -5737,7 +5766,7 @@
         <v>17</v>
       </c>
       <c r="D109" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E109" s="17">
         <v>44097</v>
@@ -5764,7 +5793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:12" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:12" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A110" s="22" t="s">
         <v>19</v>
       </c>
@@ -5775,7 +5804,7 @@
         <v>17</v>
       </c>
       <c r="D110" s="24" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E110" s="17">
         <v>44097</v>
@@ -5802,7 +5831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:12" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:12" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A111" s="22" t="s">
         <v>19</v>
       </c>
@@ -5813,7 +5842,7 @@
         <v>17</v>
       </c>
       <c r="D111" s="24" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E111" s="17">
         <v>44097</v>
@@ -5840,7 +5869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:12" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:12" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A112" s="22" t="s">
         <v>19</v>
       </c>
@@ -5851,7 +5880,7 @@
         <v>17</v>
       </c>
       <c r="D112" s="24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E112" s="17">
         <v>44098</v>
@@ -5878,7 +5907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A113" s="22" t="s">
         <v>19</v>
       </c>
@@ -5889,7 +5918,7 @@
         <v>17</v>
       </c>
       <c r="D113" s="24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E113" s="17">
         <v>44098</v>
@@ -5919,7 +5948,7 @@
       <c r="O113" s="22"/>
       <c r="P113" s="22"/>
     </row>
-    <row r="114" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A114" s="22" t="s">
         <v>19</v>
       </c>
@@ -5930,7 +5959,7 @@
         <v>17</v>
       </c>
       <c r="D114" s="24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E114" s="17">
         <v>44099</v>
@@ -5960,7 +5989,7 @@
       <c r="O114" s="22"/>
       <c r="P114" s="22"/>
     </row>
-    <row r="115" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A115" s="22" t="s">
         <v>19</v>
       </c>
@@ -5971,7 +6000,7 @@
         <v>17</v>
       </c>
       <c r="D115" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E115" s="17">
         <v>44099</v>
@@ -6001,7 +6030,7 @@
       <c r="O115" s="22"/>
       <c r="P115" s="22"/>
     </row>
-    <row r="116" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A116" s="22"/>
       <c r="B116" s="23"/>
       <c r="C116" s="24"/>
@@ -6030,9 +6059,9 @@
       <c r="O116" s="22"/>
       <c r="P116" s="22"/>
     </row>
-    <row r="117" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A117" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B117" s="23" t="s">
         <v>19</v>
@@ -6064,21 +6093,21 @@
         <v>52092009</v>
       </c>
       <c r="P117" s="22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="118" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A118" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="B118" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="C118" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D118" s="24" t="s">
         <v>166</v>
-      </c>
-      <c r="B118" s="23" t="s">
-        <v>167</v>
-      </c>
-      <c r="C118" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D118" s="24" t="s">
-        <v>168</v>
       </c>
       <c r="E118" s="17">
         <v>44099</v>
@@ -6108,10 +6137,12 @@
         <f>I96+I98+I100+I101+I102+I104+I105</f>
         <v>52092009</v>
       </c>
-      <c r="O118" s="22"/>
+      <c r="O118" s="27" t="s">
+        <v>314</v>
+      </c>
       <c r="P118" s="22"/>
     </row>
-    <row r="119" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A119" s="22"/>
       <c r="B119" s="23"/>
       <c r="C119" s="24"/>
@@ -6140,9 +6171,9 @@
       <c r="O119" s="22"/>
       <c r="P119" s="22"/>
     </row>
-    <row r="120" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A120" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B120" s="23" t="s">
         <v>19</v>
@@ -6174,21 +6205,21 @@
         <v>1074121</v>
       </c>
       <c r="P120" s="22" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="121" spans="1:16" s="6" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A121" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="B121" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C121" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D121" s="20" t="s">
         <v>171</v>
-      </c>
-      <c r="B121" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="C121" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="D121" s="20" t="s">
-        <v>173</v>
       </c>
       <c r="E121" s="8">
         <v>44118</v>
@@ -6215,16 +6246,18 @@
         <v>0</v>
       </c>
       <c r="M121" s="27" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="N121" s="20">
         <f>H118</f>
         <v>1074121</v>
       </c>
-      <c r="O121" s="27"/>
+      <c r="O121" s="27" t="s">
+        <v>314</v>
+      </c>
       <c r="P121" s="27"/>
     </row>
-    <row r="122" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A122" s="22"/>
       <c r="B122" s="23"/>
       <c r="C122" s="24"/>
@@ -6253,9 +6286,9 @@
       <c r="O122" s="22"/>
       <c r="P122" s="22"/>
     </row>
-    <row r="123" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A123" s="25" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B123" s="23" t="s">
         <v>19</v>
@@ -6287,21 +6320,21 @@
         <v>669600</v>
       </c>
       <c r="P123" s="22" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="124" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A124" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="B124" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="C124" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D124" s="24" t="s">
         <v>177</v>
-      </c>
-      <c r="B124" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="C124" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D124" s="24" t="s">
-        <v>179</v>
       </c>
       <c r="E124" s="17">
         <v>44106</v>
@@ -6331,10 +6364,12 @@
         <f>I121</f>
         <v>669600</v>
       </c>
-      <c r="O124" s="22"/>
+      <c r="O124" s="27" t="s">
+        <v>314</v>
+      </c>
       <c r="P124" s="22"/>
     </row>
-    <row r="125" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A125" s="22"/>
       <c r="B125" s="23"/>
       <c r="C125" s="24"/>
@@ -6363,9 +6398,9 @@
       <c r="O125" s="22"/>
       <c r="P125" s="22"/>
     </row>
-    <row r="126" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A126" s="25" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B126" s="23" t="s">
         <v>19</v>
@@ -6396,18 +6431,18 @@
       <c r="O126" s="22"/>
       <c r="P126" s="22"/>
     </row>
-    <row r="127" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A127" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="B127" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="C127" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D127" s="24" t="s">
         <v>181</v>
-      </c>
-      <c r="B127" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C127" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D127" s="24" t="s">
-        <v>183</v>
       </c>
       <c r="E127" s="17">
         <v>44098</v>
@@ -6437,7 +6472,7 @@
       <c r="O127" s="22"/>
       <c r="P127" s="22"/>
     </row>
-    <row r="128" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A128" s="22" t="s">
         <v>19</v>
       </c>
@@ -6448,7 +6483,7 @@
         <v>17</v>
       </c>
       <c r="D128" s="24" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E128" s="17">
         <v>44104</v>
@@ -6478,7 +6513,7 @@
       <c r="O128" s="22"/>
       <c r="P128" s="22"/>
     </row>
-    <row r="129" spans="1:13" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:13" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A129" s="22" t="s">
         <v>19</v>
       </c>
@@ -6489,7 +6524,7 @@
         <v>17</v>
       </c>
       <c r="D129" s="24" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E129" s="17">
         <v>44103</v>
@@ -6516,7 +6551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:13" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A130" s="22"/>
       <c r="B130" s="23"/>
       <c r="C130" s="24"/>
@@ -6542,9 +6577,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:13" ht="12" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:13" ht="12" hidden="1" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A131" s="25" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B131" s="23" t="s">
         <v>19</v>
@@ -6572,18 +6607,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:13" s="19" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:13" s="19" customFormat="1" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A132" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B132" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C132" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D132" s="20" t="s">
         <v>187</v>
-      </c>
-      <c r="B132" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="C132" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="D132" s="20" t="s">
-        <v>189</v>
       </c>
       <c r="E132" s="8">
         <v>44104</v>
@@ -6610,10 +6645,10 @@
         <v>0</v>
       </c>
       <c r="M132" s="11" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="133" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A133" s="22"/>
       <c r="B133" s="23"/>
       <c r="C133" s="24"/>
@@ -6639,9 +6674,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:13" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A134" s="25" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B134" s="23" t="s">
         <v>19</v>
@@ -6669,18 +6704,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:13" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:13" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A135" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="B135" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="C135" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D135" s="24" t="s">
         <v>192</v>
-      </c>
-      <c r="B135" s="23" t="s">
-        <v>193</v>
-      </c>
-      <c r="C135" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D135" s="24" t="s">
-        <v>194</v>
       </c>
       <c r="E135" s="17">
         <v>44097</v>
@@ -6707,7 +6742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:13" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:13" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A136" s="22" t="s">
         <v>19</v>
       </c>
@@ -6718,7 +6753,7 @@
         <v>17</v>
       </c>
       <c r="D136" s="24" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E136" s="17">
         <v>44103</v>
@@ -6745,7 +6780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:13" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A137" s="22"/>
       <c r="B137" s="23"/>
       <c r="C137" s="24"/>
@@ -6771,9 +6806,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:13" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A138" s="25" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B138" s="23" t="s">
         <v>19</v>
@@ -6801,18 +6836,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:13" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:13" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A139" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="B139" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="C139" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D139" s="24" t="s">
         <v>197</v>
-      </c>
-      <c r="B139" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="C139" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D139" s="24" t="s">
-        <v>199</v>
       </c>
       <c r="E139" s="17">
         <v>44111</v>
@@ -6839,7 +6874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:13" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:13" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A140" s="22" t="s">
         <v>19</v>
       </c>
@@ -6850,7 +6885,7 @@
         <v>17</v>
       </c>
       <c r="D140" s="24" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E140" s="17">
         <v>44110</v>
@@ -6877,7 +6912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:13" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:13" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A141" s="22" t="s">
         <v>19</v>
       </c>
@@ -6888,7 +6923,7 @@
         <v>17</v>
       </c>
       <c r="D141" s="24" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E141" s="17">
         <v>44114</v>
@@ -6915,7 +6950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:13" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:13" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A142" s="22" t="s">
         <v>19</v>
       </c>
@@ -6926,7 +6961,7 @@
         <v>17</v>
       </c>
       <c r="D142" s="24" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E142" s="17">
         <v>44090</v>
@@ -6953,7 +6988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:13" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:13" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A143" s="22" t="s">
         <v>19</v>
       </c>
@@ -6964,7 +6999,7 @@
         <v>17</v>
       </c>
       <c r="D143" s="24" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E143" s="17">
         <v>44096</v>
@@ -6991,7 +7026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:13" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:13" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A144" s="22" t="s">
         <v>19</v>
       </c>
@@ -7002,7 +7037,7 @@
         <v>17</v>
       </c>
       <c r="D144" s="24" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E144" s="17">
         <v>44093</v>
@@ -7029,7 +7064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A145" s="22" t="s">
         <v>19</v>
       </c>
@@ -7040,7 +7075,7 @@
         <v>17</v>
       </c>
       <c r="D145" s="24" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E145" s="17">
         <v>44092</v>
@@ -7070,7 +7105,7 @@
       <c r="O145" s="22"/>
       <c r="P145" s="22"/>
     </row>
-    <row r="146" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A146" s="22" t="s">
         <v>19</v>
       </c>
@@ -7081,7 +7116,7 @@
         <v>17</v>
       </c>
       <c r="D146" s="24" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E146" s="17">
         <v>44097</v>
@@ -7111,7 +7146,7 @@
       <c r="O146" s="22"/>
       <c r="P146" s="22"/>
     </row>
-    <row r="147" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A147" s="22" t="s">
         <v>19</v>
       </c>
@@ -7122,7 +7157,7 @@
         <v>17</v>
       </c>
       <c r="D147" s="24" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E147" s="17">
         <v>44098</v>
@@ -7152,7 +7187,7 @@
       <c r="O147" s="22"/>
       <c r="P147" s="22"/>
     </row>
-    <row r="148" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A148" s="22" t="s">
         <v>19</v>
       </c>
@@ -7163,7 +7198,7 @@
         <v>17</v>
       </c>
       <c r="D148" s="24" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E148" s="17">
         <v>44103</v>
@@ -7193,7 +7228,7 @@
       <c r="O148" s="22"/>
       <c r="P148" s="22"/>
     </row>
-    <row r="149" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A149" s="22" t="s">
         <v>19</v>
       </c>
@@ -7204,7 +7239,7 @@
         <v>17</v>
       </c>
       <c r="D149" s="24" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E149" s="17">
         <v>44102</v>
@@ -7234,7 +7269,7 @@
       <c r="O149" s="22"/>
       <c r="P149" s="22"/>
     </row>
-    <row r="150" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A150" s="22" t="s">
         <v>19</v>
       </c>
@@ -7245,7 +7280,7 @@
         <v>17</v>
       </c>
       <c r="D150" s="24" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E150" s="17">
         <v>44089</v>
@@ -7275,7 +7310,7 @@
       <c r="O150" s="22"/>
       <c r="P150" s="22"/>
     </row>
-    <row r="151" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A151" s="22" t="s">
         <v>19</v>
       </c>
@@ -7286,7 +7321,7 @@
         <v>17</v>
       </c>
       <c r="D151" s="24" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E151" s="17">
         <v>44089</v>
@@ -7316,7 +7351,7 @@
       <c r="O151" s="22"/>
       <c r="P151" s="22"/>
     </row>
-    <row r="152" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A152" s="22" t="s">
         <v>19</v>
       </c>
@@ -7327,7 +7362,7 @@
         <v>17</v>
       </c>
       <c r="D152" s="24" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E152" s="17">
         <v>44098</v>
@@ -7357,7 +7392,7 @@
       <c r="O152" s="22"/>
       <c r="P152" s="22"/>
     </row>
-    <row r="153" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A153" s="22" t="s">
         <v>19</v>
       </c>
@@ -7368,7 +7403,7 @@
         <v>17</v>
       </c>
       <c r="D153" s="24" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E153" s="17">
         <v>44104</v>
@@ -7398,7 +7433,7 @@
       <c r="O153" s="22"/>
       <c r="P153" s="22"/>
     </row>
-    <row r="154" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A154" s="22" t="s">
         <v>19</v>
       </c>
@@ -7409,7 +7444,7 @@
         <v>17</v>
       </c>
       <c r="D154" s="24" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E154" s="17">
         <v>44103</v>
@@ -7439,7 +7474,7 @@
       <c r="O154" s="22"/>
       <c r="P154" s="22"/>
     </row>
-    <row r="155" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A155" s="22"/>
       <c r="B155" s="23"/>
       <c r="C155" s="24"/>
@@ -7468,9 +7503,9 @@
       <c r="O155" s="22"/>
       <c r="P155" s="22"/>
     </row>
-    <row r="156" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A156" s="25" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B156" s="23" t="s">
         <v>19</v>
@@ -7502,21 +7537,21 @@
         <v>18089916</v>
       </c>
       <c r="P156" s="22" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="157" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A157" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="B157" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="C157" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D157" s="24" t="s">
         <v>217</v>
-      </c>
-      <c r="B157" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="C157" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D157" s="24" t="s">
-        <v>219</v>
       </c>
       <c r="E157" s="17">
         <v>44110</v>
@@ -7546,10 +7581,12 @@
         <f>I150+I151+H142+H145+H144+H143+H146+H147+H152</f>
         <v>18089916</v>
       </c>
-      <c r="O157" s="22"/>
+      <c r="O157" s="27" t="s">
+        <v>314</v>
+      </c>
       <c r="P157" s="22"/>
     </row>
-    <row r="158" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A158" s="22" t="s">
         <v>19</v>
       </c>
@@ -7560,7 +7597,7 @@
         <v>17</v>
       </c>
       <c r="D158" s="24" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E158" s="17">
         <v>44097</v>
@@ -7590,7 +7627,7 @@
       <c r="O158" s="22"/>
       <c r="P158" s="22"/>
     </row>
-    <row r="159" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A159" s="22"/>
       <c r="B159" s="23"/>
       <c r="C159" s="24"/>
@@ -7619,9 +7656,9 @@
       <c r="O159" s="22"/>
       <c r="P159" s="22"/>
     </row>
-    <row r="160" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A160" s="25" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B160" s="23" t="s">
         <v>19</v>
@@ -7653,21 +7690,21 @@
         <v>4094318</v>
       </c>
       <c r="P160" s="22" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="161" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A161" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="B161" s="23" t="s">
+        <v>222</v>
+      </c>
+      <c r="C161" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D161" s="24" t="s">
         <v>223</v>
-      </c>
-      <c r="B161" s="23" t="s">
-        <v>224</v>
-      </c>
-      <c r="C161" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D161" s="24" t="s">
-        <v>225</v>
       </c>
       <c r="E161" s="17">
         <v>44110</v>
@@ -7697,10 +7734,12 @@
         <f>H158+H157</f>
         <v>4094318</v>
       </c>
-      <c r="O161" s="22"/>
+      <c r="O161" s="27" t="s">
+        <v>314</v>
+      </c>
       <c r="P161" s="22"/>
     </row>
-    <row r="162" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A162" s="22"/>
       <c r="B162" s="23"/>
       <c r="C162" s="24"/>
@@ -7729,9 +7768,9 @@
       <c r="O162" s="22"/>
       <c r="P162" s="22"/>
     </row>
-    <row r="163" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A163" s="25" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B163" s="23" t="s">
         <v>19</v>
@@ -7762,18 +7801,18 @@
       <c r="O163" s="22"/>
       <c r="P163" s="22"/>
     </row>
-    <row r="164" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A164" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="B164" s="23" t="s">
+        <v>226</v>
+      </c>
+      <c r="C164" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D164" s="24" t="s">
         <v>227</v>
-      </c>
-      <c r="B164" s="23" t="s">
-        <v>228</v>
-      </c>
-      <c r="C164" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D164" s="24" t="s">
-        <v>229</v>
       </c>
       <c r="E164" s="17">
         <v>44102</v>
@@ -7803,7 +7842,7 @@
       <c r="O164" s="22"/>
       <c r="P164" s="22"/>
     </row>
-    <row r="165" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A165" s="22"/>
       <c r="B165" s="23"/>
       <c r="C165" s="24"/>
@@ -7832,9 +7871,9 @@
       <c r="O165" s="22"/>
       <c r="P165" s="22"/>
     </row>
-    <row r="166" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A166" s="25" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B166" s="23" t="s">
         <v>19</v>
@@ -7865,18 +7904,18 @@
       <c r="O166" s="22"/>
       <c r="P166" s="22"/>
     </row>
-    <row r="167" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A167" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="B167" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="C167" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D167" s="24" t="s">
         <v>231</v>
-      </c>
-      <c r="B167" s="23" t="s">
-        <v>232</v>
-      </c>
-      <c r="C167" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D167" s="24" t="s">
-        <v>233</v>
       </c>
       <c r="E167" s="17">
         <v>44109</v>
@@ -7906,7 +7945,7 @@
       <c r="O167" s="22"/>
       <c r="P167" s="22"/>
     </row>
-    <row r="168" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A168" s="22"/>
       <c r="B168" s="23"/>
       <c r="C168" s="24"/>
@@ -7935,9 +7974,9 @@
       <c r="O168" s="22"/>
       <c r="P168" s="22"/>
     </row>
-    <row r="169" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A169" s="25" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B169" s="23" t="s">
         <v>19</v>
@@ -7968,18 +8007,18 @@
       <c r="O169" s="22"/>
       <c r="P169" s="22"/>
     </row>
-    <row r="170" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A170" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="B170" s="23" t="s">
+        <v>234</v>
+      </c>
+      <c r="C170" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D170" s="24" t="s">
         <v>235</v>
-      </c>
-      <c r="B170" s="23" t="s">
-        <v>236</v>
-      </c>
-      <c r="C170" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D170" s="24" t="s">
-        <v>237</v>
       </c>
       <c r="E170" s="17">
         <v>44080</v>
@@ -8006,13 +8045,13 @@
         <v>0</v>
       </c>
       <c r="M170" s="10" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="N170" s="22"/>
       <c r="O170" s="22"/>
       <c r="P170" s="22"/>
     </row>
-    <row r="171" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A171" s="22"/>
       <c r="B171" s="23"/>
       <c r="C171" s="24"/>
@@ -8041,9 +8080,9 @@
       <c r="O171" s="22"/>
       <c r="P171" s="22"/>
     </row>
-    <row r="172" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A172" s="25" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B172" s="23" t="s">
         <v>19</v>
@@ -8074,18 +8113,18 @@
       <c r="O172" s="22"/>
       <c r="P172" s="22"/>
     </row>
-    <row r="173" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A173" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="B173" s="23" t="s">
+        <v>239</v>
+      </c>
+      <c r="C173" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D173" s="24" t="s">
         <v>240</v>
-      </c>
-      <c r="B173" s="23" t="s">
-        <v>241</v>
-      </c>
-      <c r="C173" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D173" s="24" t="s">
-        <v>242</v>
       </c>
       <c r="E173" s="17">
         <v>44098</v>
@@ -8115,7 +8154,7 @@
       <c r="O173" s="22"/>
       <c r="P173" s="22"/>
     </row>
-    <row r="174" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A174" s="22"/>
       <c r="B174" s="23"/>
       <c r="C174" s="24"/>
@@ -8144,9 +8183,9 @@
       <c r="O174" s="22"/>
       <c r="P174" s="22"/>
     </row>
-    <row r="175" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A175" s="25" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B175" s="23" t="s">
         <v>19</v>
@@ -8178,21 +8217,21 @@
         <v>492503</v>
       </c>
       <c r="P175" s="22" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="176" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A176" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="B176" s="23" t="s">
+        <v>244</v>
+      </c>
+      <c r="C176" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D176" s="24" t="s">
         <v>245</v>
-      </c>
-      <c r="B176" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C176" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D176" s="24" t="s">
-        <v>247</v>
       </c>
       <c r="E176" s="17">
         <v>44110</v>
@@ -8222,10 +8261,12 @@
         <f>H173</f>
         <v>492503</v>
       </c>
-      <c r="O176" s="22"/>
+      <c r="O176" s="27" t="s">
+        <v>314</v>
+      </c>
       <c r="P176" s="22"/>
     </row>
-    <row r="177" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A177" s="22"/>
       <c r="B177" s="23"/>
       <c r="C177" s="24"/>
@@ -8254,9 +8295,9 @@
       <c r="O177" s="22"/>
       <c r="P177" s="22"/>
     </row>
-    <row r="178" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A178" s="25" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B178" s="23" t="s">
         <v>19</v>
@@ -8287,18 +8328,18 @@
       <c r="O178" s="22"/>
       <c r="P178" s="22"/>
     </row>
-    <row r="179" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A179" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="B179" s="23" t="s">
+        <v>248</v>
+      </c>
+      <c r="C179" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D179" s="24" t="s">
         <v>249</v>
-      </c>
-      <c r="B179" s="23" t="s">
-        <v>250</v>
-      </c>
-      <c r="C179" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D179" s="24" t="s">
-        <v>251</v>
       </c>
       <c r="E179" s="17">
         <v>44109</v>
@@ -8328,7 +8369,7 @@
       <c r="O179" s="22"/>
       <c r="P179" s="22"/>
     </row>
-    <row r="180" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A180" s="22" t="s">
         <v>19</v>
       </c>
@@ -8339,7 +8380,7 @@
         <v>17</v>
       </c>
       <c r="D180" s="24" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E180" s="17">
         <v>44109</v>
@@ -8369,7 +8410,7 @@
       <c r="O180" s="22"/>
       <c r="P180" s="22"/>
     </row>
-    <row r="181" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A181" s="22" t="s">
         <v>19</v>
       </c>
@@ -8380,7 +8421,7 @@
         <v>17</v>
       </c>
       <c r="D181" s="24" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E181" s="17">
         <v>44111</v>
@@ -8410,7 +8451,7 @@
       <c r="O181" s="22"/>
       <c r="P181" s="22"/>
     </row>
-    <row r="182" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A182" s="22" t="s">
         <v>19</v>
       </c>
@@ -8421,7 +8462,7 @@
         <v>17</v>
       </c>
       <c r="D182" s="24" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E182" s="17">
         <v>44118</v>
@@ -8451,7 +8492,7 @@
       <c r="O182" s="22"/>
       <c r="P182" s="22"/>
     </row>
-    <row r="183" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A183" s="22" t="s">
         <v>19</v>
       </c>
@@ -8462,7 +8503,7 @@
         <v>17</v>
       </c>
       <c r="D183" s="24" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E183" s="17">
         <v>44118</v>
@@ -8492,7 +8533,7 @@
       <c r="O183" s="22"/>
       <c r="P183" s="22"/>
     </row>
-    <row r="184" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A184" s="22" t="s">
         <v>19</v>
       </c>
@@ -8503,7 +8544,7 @@
         <v>17</v>
       </c>
       <c r="D184" s="24" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E184" s="17">
         <v>44090</v>
@@ -8533,7 +8574,7 @@
       <c r="O184" s="22"/>
       <c r="P184" s="22"/>
     </row>
-    <row r="185" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A185" s="22" t="s">
         <v>19</v>
       </c>
@@ -8544,7 +8585,7 @@
         <v>17</v>
       </c>
       <c r="D185" s="24" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E185" s="17">
         <v>44098</v>
@@ -8574,7 +8615,7 @@
       <c r="O185" s="22"/>
       <c r="P185" s="22"/>
     </row>
-    <row r="186" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A186" s="22" t="s">
         <v>19</v>
       </c>
@@ -8585,7 +8626,7 @@
         <v>17</v>
       </c>
       <c r="D186" s="24" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E186" s="17">
         <v>44099</v>
@@ -8615,7 +8656,7 @@
       <c r="O186" s="22"/>
       <c r="P186" s="22"/>
     </row>
-    <row r="187" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A187" s="22"/>
       <c r="B187" s="23"/>
       <c r="C187" s="24"/>
@@ -8644,9 +8685,9 @@
       <c r="O187" s="22"/>
       <c r="P187" s="22"/>
     </row>
-    <row r="188" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A188" s="25" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B188" s="23" t="s">
         <v>19</v>
@@ -8678,21 +8719,21 @@
         <v>6013778</v>
       </c>
       <c r="P188" s="22" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="189" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A189" s="22" t="s">
+        <v>258</v>
+      </c>
+      <c r="B189" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="C189" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D189" s="24" t="s">
         <v>260</v>
-      </c>
-      <c r="B189" s="23" t="s">
-        <v>261</v>
-      </c>
-      <c r="C189" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D189" s="24" t="s">
-        <v>262</v>
       </c>
       <c r="E189" s="17">
         <v>44120</v>
@@ -8722,10 +8763,12 @@
         <f>I182+H184</f>
         <v>6013778</v>
       </c>
-      <c r="O189" s="22"/>
+      <c r="O189" s="27" t="s">
+        <v>314</v>
+      </c>
       <c r="P189" s="22"/>
     </row>
-    <row r="190" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A190" s="22"/>
       <c r="B190" s="23"/>
       <c r="C190" s="24"/>
@@ -8754,9 +8797,9 @@
       <c r="O190" s="22"/>
       <c r="P190" s="22"/>
     </row>
-    <row r="191" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A191" s="25" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B191" s="23" t="s">
         <v>19</v>
@@ -8788,21 +8831,21 @@
         <v>4031339</v>
       </c>
       <c r="P191" s="22" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="192" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A192" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="B192" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="C192" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D192" s="24" t="s">
         <v>265</v>
-      </c>
-      <c r="B192" s="23" t="s">
-        <v>266</v>
-      </c>
-      <c r="C192" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D192" s="24" t="s">
-        <v>267</v>
       </c>
       <c r="E192" s="17">
         <v>44105</v>
@@ -8832,10 +8875,12 @@
         <f>H189</f>
         <v>4031339</v>
       </c>
-      <c r="O192" s="22"/>
+      <c r="O192" s="27" t="s">
+        <v>313</v>
+      </c>
       <c r="P192" s="22"/>
     </row>
-    <row r="193" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A193" s="22" t="s">
         <v>19</v>
       </c>
@@ -8846,7 +8891,7 @@
         <v>17</v>
       </c>
       <c r="D193" s="24" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E193" s="17">
         <v>44105</v>
@@ -8876,7 +8921,7 @@
       <c r="O193" s="22"/>
       <c r="P193" s="22"/>
     </row>
-    <row r="194" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A194" s="22" t="s">
         <v>19</v>
       </c>
@@ -8887,7 +8932,7 @@
         <v>17</v>
       </c>
       <c r="D194" s="24" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E194" s="17">
         <v>44112</v>
@@ -8917,7 +8962,7 @@
       <c r="O194" s="22"/>
       <c r="P194" s="22"/>
     </row>
-    <row r="195" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A195" s="22" t="s">
         <v>19</v>
       </c>
@@ -8928,7 +8973,7 @@
         <v>17</v>
       </c>
       <c r="D195" s="24" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E195" s="17">
         <v>44092</v>
@@ -8958,7 +9003,7 @@
       <c r="O195" s="22"/>
       <c r="P195" s="22"/>
     </row>
-    <row r="196" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A196" s="22" t="s">
         <v>19</v>
       </c>
@@ -8969,7 +9014,7 @@
         <v>17</v>
       </c>
       <c r="D196" s="24" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E196" s="17">
         <v>44092</v>
@@ -8999,7 +9044,7 @@
       <c r="O196" s="22"/>
       <c r="P196" s="22"/>
     </row>
-    <row r="197" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A197" s="22" t="s">
         <v>19</v>
       </c>
@@ -9010,7 +9055,7 @@
         <v>17</v>
       </c>
       <c r="D197" s="24" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E197" s="17">
         <v>44096</v>
@@ -9040,7 +9085,7 @@
       <c r="O197" s="22"/>
       <c r="P197" s="22"/>
     </row>
-    <row r="198" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A198" s="22" t="s">
         <v>19</v>
       </c>
@@ -9051,7 +9096,7 @@
         <v>17</v>
       </c>
       <c r="D198" s="24" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E198" s="17">
         <v>44099</v>
@@ -9081,7 +9126,7 @@
       <c r="O198" s="22"/>
       <c r="P198" s="22"/>
     </row>
-    <row r="199" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A199" s="22"/>
       <c r="B199" s="23"/>
       <c r="C199" s="24"/>
@@ -9110,9 +9155,9 @@
       <c r="O199" s="22"/>
       <c r="P199" s="22"/>
     </row>
-    <row r="200" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A200" s="25" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B200" s="23" t="s">
         <v>19</v>
@@ -9144,12 +9189,12 @@
         <v>11817175</v>
       </c>
       <c r="P200" s="22" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="201" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A201" s="25" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B201" s="23" t="s">
         <v>19</v>
@@ -9186,7 +9231,7 @@
         <f>H195+H196+H197+H198</f>
         <v>11817175</v>
       </c>
-      <c r="O201" s="22"/>
+      <c r="O201" s="27"/>
       <c r="P201" s="22"/>
     </row>
     <row r="202" spans="1:16" x14ac:dyDescent="0.2">
@@ -9219,7 +9264,7 @@
     </row>
     <row r="205" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A205" s="22" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B205" s="21"/>
       <c r="C205" s="21"/>
@@ -9245,7 +9290,7 @@
     </row>
     <row r="206" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A206" s="22" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B206" s="23"/>
       <c r="C206" s="24"/>
@@ -9269,7 +9314,7 @@
     </row>
     <row r="207" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A207" s="22" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B207" s="23"/>
       <c r="C207" s="24"/>
@@ -9291,7 +9336,7 @@
     </row>
     <row r="208" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A208" s="22" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B208" s="23"/>
       <c r="C208" s="24"/>
@@ -9310,7 +9355,7 @@
     </row>
     <row r="209" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A209" s="22" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B209" s="23"/>
       <c r="C209" s="24"/>
@@ -9328,7 +9373,7 @@
     </row>
     <row r="210" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A210" s="22" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B210" s="23"/>
       <c r="C210" s="24"/>
@@ -9340,7 +9385,7 @@
         <v>184142618</v>
       </c>
       <c r="H210" s="24" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I210" s="24"/>
       <c r="J210" s="24"/>
@@ -9349,7 +9394,7 @@
     </row>
     <row r="211" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A211" s="22" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B211" s="23"/>
       <c r="C211" s="24"/>
@@ -9367,7 +9412,7 @@
     </row>
     <row r="214" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A214" s="25" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B214" s="23"/>
       <c r="C214" s="24"/>
@@ -9387,6 +9432,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:P201" xr:uid="{B9716568-C4F4-4EC6-BC6F-AF9B6A1AD659}">
+    <filterColumn colId="13">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -9497,13 +9549,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B5" s="24" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D5" s="17">
         <v>44077</v>
@@ -9530,7 +9582,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -9539,7 +9591,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D6" s="17">
         <v>44083</v>
@@ -9573,7 +9625,7 @@
         <v>17</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D7" s="17">
         <v>44068</v>
@@ -9607,7 +9659,7 @@
         <v>17</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D8" s="17">
         <v>44049</v>
@@ -9663,7 +9715,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B10" s="21"/>
       <c r="C10" s="17"/>
@@ -9756,21 +9808,21 @@
         <v>11</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
+        <v>291</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>292</v>
+      </c>
+      <c r="C3" s="24" t="s">
         <v>293</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="D3" s="24" t="s">
         <v>294</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>295</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>296</v>
       </c>
       <c r="E3" s="17">
         <v>44046</v>
@@ -9797,7 +9849,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="22" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -9811,7 +9863,7 @@
         <v>17</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E4" s="17">
         <v>44049</v>
@@ -9850,7 +9902,7 @@
         <v>17</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E5" s="17">
         <v>44076</v>
@@ -9886,10 +9938,10 @@
         <v>19</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E6" s="17">
         <v>44084</v>
@@ -9928,7 +9980,7 @@
         <v>17</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E7" s="17">
         <v>44078</v>
@@ -9964,10 +10016,10 @@
         <v>19</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E8" s="17">
         <v>43957</v>
@@ -9994,7 +10046,7 @@
         <v>9975000</v>
       </c>
       <c r="M8" s="15" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -10005,10 +10057,10 @@
         <v>19</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E9" s="17">
         <v>43959</v>
@@ -10044,10 +10096,10 @@
         <v>19</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E10" s="17">
         <v>43962</v>
@@ -10086,7 +10138,7 @@
         <v>17</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E11" s="17">
         <v>43998</v>
@@ -10125,7 +10177,7 @@
         <v>17</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E12" s="17">
         <v>44022</v>
@@ -10161,10 +10213,10 @@
         <v>19</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E13" s="17">
         <v>43964</v>
@@ -10200,10 +10252,10 @@
         <v>19</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E14" s="17">
         <v>44042</v>
@@ -10239,10 +10291,10 @@
         <v>19</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E15" s="17">
         <v>44043</v>
@@ -10278,10 +10330,10 @@
         <v>19</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E16" s="17">
         <v>43901</v>
@@ -10317,10 +10369,10 @@
         <v>19</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E17" s="17">
         <v>43902</v>
@@ -10377,7 +10429,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="25" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B19" s="23" t="s">
         <v>19</v>
@@ -10430,6 +10482,52 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <uuca xmlns="6fc73c7f-b275-407f-b566-8650e0038fa7" xsi:nil="true"/>
+    <VERIFICADAVSCONTABILIDAD xmlns="6fc73c7f-b275-407f-b566-8650e0038fa7">Verificada</VERIFICADAVSCONTABILIDAD>
+    <verificada xmlns="6fc73c7f-b275-407f-b566-8650e0038fa7" xsi:nil="true"/>
+    <SharedWithUsers xmlns="e351c5d8-61e1-41b6-84d8-e536a78b6c0c">
+      <UserInfo>
+        <DisplayName>Sheylla Jinette</DisplayName>
+        <AccountId>15</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Daniel Andres Bueno Salazar</DisplayName>
+        <AccountId>20</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Tesoreria Centronet</DisplayName>
+        <AccountId>37</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Lady Tamayo</DisplayName>
+        <AccountId>11</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Alejandro Jimenez Rodriguez</DisplayName>
+        <AccountId>16</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B0A9EB854EEA5F40B987FCB721535166" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="0a2f17941310ab99bd76ff2788221c8e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e351c5d8-61e1-41b6-84d8-e536a78b6c0c" xmlns:ns3="6fc73c7f-b275-407f-b566-8650e0038fa7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1a092763a2126285159078240ff12f4e" ns2:_="" ns3:_="">
     <xsd:import namespace="e351c5d8-61e1-41b6-84d8-e536a78b6c0c"/>
@@ -10648,53 +10746,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <uuca xmlns="6fc73c7f-b275-407f-b566-8650e0038fa7" xsi:nil="true"/>
-    <VERIFICADAVSCONTABILIDAD xmlns="6fc73c7f-b275-407f-b566-8650e0038fa7">Verificada</VERIFICADAVSCONTABILIDAD>
-    <verificada xmlns="6fc73c7f-b275-407f-b566-8650e0038fa7" xsi:nil="true"/>
-    <SharedWithUsers xmlns="e351c5d8-61e1-41b6-84d8-e536a78b6c0c">
-      <UserInfo>
-        <DisplayName>Sheylla Jinette</DisplayName>
-        <AccountId>15</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Daniel Andres Bueno Salazar</DisplayName>
-        <AccountId>20</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Tesoreria Centronet</DisplayName>
-        <AccountId>37</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Lady Tamayo</DisplayName>
-        <AccountId>11</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Alejandro Jimenez Rodriguez</DisplayName>
-        <AccountId>16</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90182CCF-3801-4877-87A2-5B157A562960}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6fc73c7f-b275-407f-b566-8650e0038fa7"/>
+    <ds:schemaRef ds:uri="e351c5d8-61e1-41b6-84d8-e536a78b6c0c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{846F462C-5710-4CBF-99A1-C0D3749D205F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29AAA06B-57BD-4169-B95F-036023BB1644}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10711,23 +10782,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90182CCF-3801-4877-87A2-5B157A562960}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6fc73c7f-b275-407f-b566-8650e0038fa7"/>
-    <ds:schemaRef ds:uri="e351c5d8-61e1-41b6-84d8-e536a78b6c0c"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{846F462C-5710-4CBF-99A1-C0D3749D205F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
version 1.0 pruenas: ok
</commit_message>
<xml_diff>
--- a/reporte de cuentas por pagar.xlsx
+++ b/reporte de cuentas por pagar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Diana\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC2AAF3-C6BC-47CA-8068-36FF1C424CE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC0DBBD-1729-436B-B7FE-8B4F101F8536}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="317">
   <si>
     <t>Nombres</t>
   </si>
@@ -985,6 +985,9 @@
   </si>
   <si>
     <t>NIT 1143940723 - 2</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -1071,7 +1074,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1112,6 +1115,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda [0] 2" xfId="2" xr:uid="{499486D7-B39C-4A07-A925-7B8DEF32608F}"/>
@@ -1529,10 +1533,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Hoja1" filterMode="1"/>
+  <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P214"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="4" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1602,7 +1608,7 @@
       </c>
       <c r="P1" s="22"/>
     </row>
-    <row r="2" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
         <v>15</v>
       </c>
@@ -1643,7 +1649,7 @@
       <c r="O2" s="22"/>
       <c r="P2" s="22"/>
     </row>
-    <row r="3" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
         <v>19</v>
       </c>
@@ -1684,7 +1690,7 @@
       <c r="O3" s="22"/>
       <c r="P3" s="22"/>
     </row>
-    <row r="4" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
         <v>19</v>
       </c>
@@ -1725,7 +1731,7 @@
       <c r="O4" s="22"/>
       <c r="P4" s="22"/>
     </row>
-    <row r="5" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A5" s="22"/>
       <c r="B5" s="23"/>
       <c r="C5" s="24"/>
@@ -1754,7 +1760,7 @@
       <c r="O5" s="22"/>
       <c r="P5" s="22"/>
     </row>
-    <row r="6" spans="1:16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>22</v>
       </c>
@@ -1787,7 +1793,7 @@
       <c r="O6" s="22"/>
       <c r="P6" s="22"/>
     </row>
-    <row r="7" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
         <v>23</v>
       </c>
@@ -1828,7 +1834,7 @@
       <c r="O7" s="22"/>
       <c r="P7" s="22"/>
     </row>
-    <row r="8" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
         <v>19</v>
       </c>
@@ -1869,7 +1875,7 @@
       <c r="O8" s="22"/>
       <c r="P8" s="22"/>
     </row>
-    <row r="9" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24"/>
@@ -1898,7 +1904,7 @@
       <c r="O9" s="22"/>
       <c r="P9" s="22"/>
     </row>
-    <row r="10" spans="1:16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
         <v>27</v>
       </c>
@@ -1931,7 +1937,7 @@
       <c r="O10" s="22"/>
       <c r="P10" s="22"/>
     </row>
-    <row r="11" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A11" s="22" t="s">
         <v>28</v>
       </c>
@@ -1972,7 +1978,7 @@
       <c r="O11" s="22"/>
       <c r="P11" s="22"/>
     </row>
-    <row r="12" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A12" s="22" t="s">
         <v>19</v>
       </c>
@@ -2013,7 +2019,7 @@
       <c r="O12" s="22"/>
       <c r="P12" s="22"/>
     </row>
-    <row r="13" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A13" s="22" t="s">
         <v>19</v>
       </c>
@@ -2054,7 +2060,7 @@
       <c r="O13" s="22"/>
       <c r="P13" s="22"/>
     </row>
-    <row r="14" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A14" s="22"/>
       <c r="B14" s="23"/>
       <c r="C14" s="24"/>
@@ -2083,7 +2089,7 @@
       <c r="O14" s="22"/>
       <c r="P14" s="22"/>
     </row>
-    <row r="15" spans="1:16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="s">
         <v>33</v>
       </c>
@@ -2165,11 +2171,11 @@
         <v>2359386</v>
       </c>
       <c r="O16" s="27" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="P16" s="27"/>
     </row>
-    <row r="17" spans="1:16" s="6" customFormat="1" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" s="6" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A17" s="27" t="s">
         <v>19</v>
       </c>
@@ -2213,7 +2219,7 @@
       <c r="O17" s="27"/>
       <c r="P17" s="27"/>
     </row>
-    <row r="18" spans="1:16" s="6" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" s="6" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A18" s="27"/>
       <c r="B18" s="7"/>
       <c r="C18" s="20"/>
@@ -2243,7 +2249,7 @@
       <c r="O18" s="27"/>
       <c r="P18" s="27"/>
     </row>
-    <row r="19" spans="1:16" s="6" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" s="6" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
         <v>41</v>
       </c>
@@ -2323,11 +2329,11 @@
         <v>525870</v>
       </c>
       <c r="O20" s="27" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="P20" s="22"/>
     </row>
-    <row r="21" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A21" s="22"/>
       <c r="B21" s="23"/>
       <c r="C21" s="24"/>
@@ -2356,7 +2362,7 @@
       <c r="O21" s="22"/>
       <c r="P21" s="22"/>
     </row>
-    <row r="22" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A22" s="25" t="s">
         <v>46</v>
       </c>
@@ -2397,7 +2403,7 @@
       <c r="A23" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="30" t="s">
         <v>315</v>
       </c>
       <c r="C23" s="24" t="s">
@@ -2438,11 +2444,11 @@
         <v>87451</v>
       </c>
       <c r="O23" s="27" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="P23" s="22"/>
     </row>
-    <row r="24" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A24" s="22"/>
       <c r="B24" s="23"/>
       <c r="C24" s="24"/>
@@ -2471,7 +2477,7 @@
       <c r="O24" s="22"/>
       <c r="P24" s="22"/>
     </row>
-    <row r="25" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A25" s="25" t="s">
         <v>51</v>
       </c>
@@ -2551,11 +2557,11 @@
         <v>84300</v>
       </c>
       <c r="O26" s="27" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="P26" s="27"/>
     </row>
-    <row r="27" spans="1:16" s="6" customFormat="1" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" s="6" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A27" s="27" t="s">
         <v>19</v>
       </c>
@@ -2597,7 +2603,7 @@
       <c r="O27" s="27"/>
       <c r="P27" s="27"/>
     </row>
-    <row r="28" spans="1:16" s="6" customFormat="1" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" s="6" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A28" s="27" t="s">
         <v>19</v>
       </c>
@@ -2639,7 +2645,7 @@
       <c r="O28" s="27"/>
       <c r="P28" s="27"/>
     </row>
-    <row r="29" spans="1:16" s="6" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" s="6" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A29" s="27"/>
       <c r="B29" s="7"/>
       <c r="C29" s="20"/>
@@ -2669,7 +2675,7 @@
       <c r="O29" s="27"/>
       <c r="P29" s="27"/>
     </row>
-    <row r="30" spans="1:16" s="6" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" s="6" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>58</v>
       </c>
@@ -2745,11 +2751,11 @@
         <v>193970</v>
       </c>
       <c r="O31" s="27" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="P31" s="22"/>
     </row>
-    <row r="32" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A32" s="22" t="s">
         <v>19</v>
       </c>
@@ -2790,7 +2796,7 @@
       <c r="O32" s="22"/>
       <c r="P32" s="22"/>
     </row>
-    <row r="33" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A33" s="22"/>
       <c r="B33" s="23"/>
       <c r="C33" s="24"/>
@@ -2819,7 +2825,7 @@
       <c r="O33" s="22"/>
       <c r="P33" s="22"/>
     </row>
-    <row r="34" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A34" s="25" t="s">
         <v>63</v>
       </c>
@@ -2852,7 +2858,7 @@
       <c r="O34" s="22"/>
       <c r="P34" s="22"/>
     </row>
-    <row r="35" spans="1:16" s="6" customFormat="1" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" s="6" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A35" s="27" t="s">
         <v>64</v>
       </c>
@@ -2894,7 +2900,7 @@
       <c r="O35" s="27"/>
       <c r="P35" s="27"/>
     </row>
-    <row r="36" spans="1:16" s="6" customFormat="1" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" s="6" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A36" s="27"/>
       <c r="B36" s="7"/>
       <c r="C36" s="20"/>
@@ -2924,7 +2930,7 @@
       <c r="O36" s="27"/>
       <c r="P36" s="27"/>
     </row>
-    <row r="37" spans="1:16" s="6" customFormat="1" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" s="6" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
         <v>67</v>
       </c>
@@ -3007,11 +3013,11 @@
         <v>97991</v>
       </c>
       <c r="O38" s="27" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="P38" s="22"/>
     </row>
-    <row r="39" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A39" s="22"/>
       <c r="B39" s="23"/>
       <c r="C39" s="24"/>
@@ -3040,7 +3046,7 @@
       <c r="O39" s="22"/>
       <c r="P39" s="22"/>
     </row>
-    <row r="40" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A40" s="25" t="s">
         <v>73</v>
       </c>
@@ -3076,7 +3082,7 @@
       <c r="O40" s="22"/>
       <c r="P40" s="22"/>
     </row>
-    <row r="41" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A41" s="22" t="s">
         <v>75</v>
       </c>
@@ -3117,7 +3123,7 @@
       <c r="O41" s="22"/>
       <c r="P41" s="22"/>
     </row>
-    <row r="42" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A42" s="22"/>
       <c r="B42" s="23"/>
       <c r="C42" s="24"/>
@@ -3146,7 +3152,7 @@
       <c r="O42" s="22"/>
       <c r="P42" s="22"/>
     </row>
-    <row r="43" spans="1:16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A43" s="25" t="s">
         <v>78</v>
       </c>
@@ -3223,11 +3229,11 @@
         <v>172500</v>
       </c>
       <c r="O44" s="27" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="P44" s="22"/>
     </row>
-    <row r="45" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A45" s="22" t="s">
         <v>19</v>
       </c>
@@ -3268,7 +3274,7 @@
       <c r="O45" s="22"/>
       <c r="P45" s="22"/>
     </row>
-    <row r="46" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A46" s="22" t="s">
         <v>19</v>
       </c>
@@ -3309,7 +3315,7 @@
       <c r="O46" s="22"/>
       <c r="P46" s="22"/>
     </row>
-    <row r="47" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A47" s="22" t="s">
         <v>19</v>
       </c>
@@ -3350,7 +3356,7 @@
       <c r="O47" s="22"/>
       <c r="P47" s="22"/>
     </row>
-    <row r="48" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A48" s="22" t="s">
         <v>19</v>
       </c>
@@ -3391,7 +3397,7 @@
       <c r="O48" s="22"/>
       <c r="P48" s="22"/>
     </row>
-    <row r="49" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A49" s="22"/>
       <c r="B49" s="23"/>
       <c r="C49" s="24"/>
@@ -3420,7 +3426,7 @@
       <c r="O49" s="22"/>
       <c r="P49" s="22"/>
     </row>
-    <row r="50" spans="1:16" ht="12" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" ht="12" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A50" s="25" t="s">
         <v>86</v>
       </c>
@@ -3500,11 +3506,11 @@
         <v>1819546</v>
       </c>
       <c r="O51" s="27" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="P51" s="27"/>
     </row>
-    <row r="52" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A52" s="22" t="s">
         <v>19</v>
       </c>
@@ -3545,7 +3551,7 @@
       <c r="O52" s="22"/>
       <c r="P52" s="22"/>
     </row>
-    <row r="53" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A53" s="22" t="s">
         <v>19</v>
       </c>
@@ -3586,7 +3592,7 @@
       <c r="O53" s="22"/>
       <c r="P53" s="22"/>
     </row>
-    <row r="54" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A54" s="22" t="s">
         <v>19</v>
       </c>
@@ -3627,7 +3633,7 @@
       <c r="O54" s="22"/>
       <c r="P54" s="22"/>
     </row>
-    <row r="55" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A55" s="22" t="s">
         <v>19</v>
       </c>
@@ -3668,7 +3674,7 @@
       <c r="O55" s="22"/>
       <c r="P55" s="22"/>
     </row>
-    <row r="56" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A56" s="22" t="s">
         <v>19</v>
       </c>
@@ -3709,7 +3715,7 @@
       <c r="O56" s="22"/>
       <c r="P56" s="22"/>
     </row>
-    <row r="57" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A57" s="22" t="s">
         <v>19</v>
       </c>
@@ -3750,7 +3756,7 @@
       <c r="O57" s="22"/>
       <c r="P57" s="22"/>
     </row>
-    <row r="58" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A58" s="22" t="s">
         <v>19</v>
       </c>
@@ -3791,7 +3797,7 @@
       <c r="O58" s="22"/>
       <c r="P58" s="22"/>
     </row>
-    <row r="59" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A59" s="22" t="s">
         <v>19</v>
       </c>
@@ -3832,7 +3838,7 @@
       <c r="O59" s="22"/>
       <c r="P59" s="22"/>
     </row>
-    <row r="60" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A60" s="22" t="s">
         <v>19</v>
       </c>
@@ -3873,7 +3879,7 @@
       <c r="O60" s="22"/>
       <c r="P60" s="22"/>
     </row>
-    <row r="61" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A61" s="22" t="s">
         <v>19</v>
       </c>
@@ -3914,7 +3920,7 @@
       <c r="O61" s="22"/>
       <c r="P61" s="22"/>
     </row>
-    <row r="62" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A62" s="22" t="s">
         <v>19</v>
       </c>
@@ -3955,7 +3961,7 @@
       <c r="O62" s="22"/>
       <c r="P62" s="22"/>
     </row>
-    <row r="63" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A63" s="22" t="s">
         <v>19</v>
       </c>
@@ -3996,7 +4002,7 @@
       <c r="O63" s="22"/>
       <c r="P63" s="22"/>
     </row>
-    <row r="64" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A64" s="22" t="s">
         <v>19</v>
       </c>
@@ -4037,7 +4043,7 @@
       <c r="O64" s="22"/>
       <c r="P64" s="22"/>
     </row>
-    <row r="65" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A65" s="22" t="s">
         <v>19</v>
       </c>
@@ -4078,7 +4084,7 @@
       <c r="O65" s="22"/>
       <c r="P65" s="22"/>
     </row>
-    <row r="66" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A66" s="22" t="s">
         <v>19</v>
       </c>
@@ -4119,7 +4125,7 @@
       <c r="O66" s="22"/>
       <c r="P66" s="22"/>
     </row>
-    <row r="67" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A67" s="22" t="s">
         <v>19</v>
       </c>
@@ -4160,7 +4166,7 @@
       <c r="O67" s="22"/>
       <c r="P67" s="22"/>
     </row>
-    <row r="68" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A68" s="22" t="s">
         <v>19</v>
       </c>
@@ -4201,7 +4207,7 @@
       <c r="O68" s="22"/>
       <c r="P68" s="22"/>
     </row>
-    <row r="69" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A69" s="22" t="s">
         <v>19</v>
       </c>
@@ -4242,7 +4248,7 @@
       <c r="O69" s="22"/>
       <c r="P69" s="22"/>
     </row>
-    <row r="70" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A70" s="22"/>
       <c r="B70" s="23"/>
       <c r="C70" s="24"/>
@@ -4272,7 +4278,7 @@
       <c r="O70" s="22"/>
       <c r="P70" s="22"/>
     </row>
-    <row r="71" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A71" s="25" t="s">
         <v>109</v>
       </c>
@@ -4351,11 +4357,11 @@
         <v>9952604</v>
       </c>
       <c r="O72" s="27" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="P72" s="22"/>
     </row>
-    <row r="73" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A73" s="22" t="s">
         <v>19</v>
       </c>
@@ -4396,7 +4402,7 @@
       <c r="O73" s="22"/>
       <c r="P73" s="22"/>
     </row>
-    <row r="74" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A74" s="22" t="s">
         <v>19</v>
       </c>
@@ -4437,7 +4443,7 @@
       <c r="O74" s="22"/>
       <c r="P74" s="22"/>
     </row>
-    <row r="75" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A75" s="22" t="s">
         <v>19</v>
       </c>
@@ -4478,7 +4484,7 @@
       <c r="O75" s="22"/>
       <c r="P75" s="22"/>
     </row>
-    <row r="76" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A76" s="22" t="s">
         <v>19</v>
       </c>
@@ -4519,7 +4525,7 @@
       <c r="O76" s="22"/>
       <c r="P76" s="22"/>
     </row>
-    <row r="77" spans="1:16" ht="38.25" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16" ht="38.25" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A77" s="22" t="s">
         <v>19</v>
       </c>
@@ -4563,7 +4569,7 @@
       <c r="O77" s="22"/>
       <c r="P77" s="22"/>
     </row>
-    <row r="78" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A78" s="22" t="s">
         <v>19</v>
       </c>
@@ -4604,7 +4610,7 @@
       <c r="O78" s="22"/>
       <c r="P78" s="22"/>
     </row>
-    <row r="79" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A79" s="22" t="s">
         <v>19</v>
       </c>
@@ -4645,7 +4651,7 @@
       <c r="O79" s="22"/>
       <c r="P79" s="22"/>
     </row>
-    <row r="80" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A80" s="22" t="s">
         <v>19</v>
       </c>
@@ -4686,7 +4692,7 @@
       <c r="O80" s="22"/>
       <c r="P80" s="22"/>
     </row>
-    <row r="81" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A81" s="22" t="s">
         <v>19</v>
       </c>
@@ -4727,7 +4733,7 @@
       <c r="O81" s="22"/>
       <c r="P81" s="22"/>
     </row>
-    <row r="82" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A82" s="22" t="s">
         <v>19</v>
       </c>
@@ -4771,7 +4777,7 @@
       <c r="O82" s="22"/>
       <c r="P82" s="22"/>
     </row>
-    <row r="83" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A83" s="22"/>
       <c r="B83" s="23"/>
       <c r="C83" s="24"/>
@@ -4800,7 +4806,7 @@
       <c r="O83" s="22"/>
       <c r="P83" s="22"/>
     </row>
-    <row r="84" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A84" s="25" t="s">
         <v>126</v>
       </c>
@@ -4879,11 +4885,11 @@
         <v>4407849</v>
       </c>
       <c r="O85" s="27" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="P85" s="22"/>
     </row>
-    <row r="86" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A86" s="22" t="s">
         <v>19</v>
       </c>
@@ -4924,7 +4930,7 @@
       <c r="O86" s="22"/>
       <c r="P86" s="22"/>
     </row>
-    <row r="87" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A87" s="22" t="s">
         <v>19</v>
       </c>
@@ -4965,7 +4971,7 @@
       <c r="O87" s="22"/>
       <c r="P87" s="22"/>
     </row>
-    <row r="88" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A88" s="22" t="s">
         <v>19</v>
       </c>
@@ -5006,7 +5012,7 @@
       <c r="O88" s="22"/>
       <c r="P88" s="22"/>
     </row>
-    <row r="89" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A89" s="22"/>
       <c r="B89" s="23"/>
       <c r="C89" s="24"/>
@@ -5035,7 +5041,7 @@
       <c r="O89" s="22"/>
       <c r="P89" s="22"/>
     </row>
-    <row r="90" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A90" s="25" t="s">
         <v>134</v>
       </c>
@@ -5068,7 +5074,7 @@
       <c r="O90" s="22"/>
       <c r="P90" s="22"/>
     </row>
-    <row r="91" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A91" s="22" t="s">
         <v>135</v>
       </c>
@@ -5109,7 +5115,7 @@
       <c r="O91" s="22"/>
       <c r="P91" s="22"/>
     </row>
-    <row r="92" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A92" s="22"/>
       <c r="B92" s="23"/>
       <c r="C92" s="24"/>
@@ -5138,7 +5144,7 @@
       <c r="O92" s="22"/>
       <c r="P92" s="22"/>
     </row>
-    <row r="93" spans="1:16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A93" s="25" t="s">
         <v>138</v>
       </c>
@@ -5171,7 +5177,7 @@
       <c r="O93" s="22"/>
       <c r="P93" s="22"/>
     </row>
-    <row r="94" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A94" s="22" t="s">
         <v>139</v>
       </c>
@@ -5212,7 +5218,7 @@
       <c r="O94" s="22"/>
       <c r="P94" s="22"/>
     </row>
-    <row r="95" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A95" s="22" t="s">
         <v>19</v>
       </c>
@@ -5253,7 +5259,7 @@
       <c r="O95" s="22"/>
       <c r="P95" s="22"/>
     </row>
-    <row r="96" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A96" s="22" t="s">
         <v>19</v>
       </c>
@@ -5294,7 +5300,7 @@
       <c r="O96" s="22"/>
       <c r="P96" s="22"/>
     </row>
-    <row r="97" spans="1:12" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:12" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A97" s="22" t="s">
         <v>19</v>
       </c>
@@ -5332,7 +5338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:12" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:12" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A98" s="22" t="s">
         <v>19</v>
       </c>
@@ -5370,7 +5376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:12" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:12" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A99" s="22" t="s">
         <v>19</v>
       </c>
@@ -5408,7 +5414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:12" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:12" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A100" s="22" t="s">
         <v>19</v>
       </c>
@@ -5446,7 +5452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:12" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:12" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A101" s="22" t="s">
         <v>19</v>
       </c>
@@ -5484,7 +5490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:12" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:12" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A102" s="22" t="s">
         <v>19</v>
       </c>
@@ -5522,7 +5528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:12" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:12" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A103" s="22" t="s">
         <v>19</v>
       </c>
@@ -5560,7 +5566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:12" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:12" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A104" s="22" t="s">
         <v>19</v>
       </c>
@@ -5598,7 +5604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:12" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:12" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A105" s="22" t="s">
         <v>19</v>
       </c>
@@ -5636,7 +5642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:12" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:12" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A106" s="22" t="s">
         <v>19</v>
       </c>
@@ -5674,7 +5680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:12" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:12" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A107" s="22" t="s">
         <v>19</v>
       </c>
@@ -5712,7 +5718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:12" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:12" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A108" s="22" t="s">
         <v>19</v>
       </c>
@@ -5750,7 +5756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:12" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:12" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A109" s="22" t="s">
         <v>19</v>
       </c>
@@ -5788,7 +5794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:12" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:12" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A110" s="22" t="s">
         <v>19</v>
       </c>
@@ -5826,7 +5832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:12" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:12" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A111" s="22" t="s">
         <v>19</v>
       </c>
@@ -5864,7 +5870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:12" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:12" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A112" s="22" t="s">
         <v>19</v>
       </c>
@@ -5902,7 +5908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A113" s="22" t="s">
         <v>19</v>
       </c>
@@ -5943,7 +5949,7 @@
       <c r="O113" s="22"/>
       <c r="P113" s="22"/>
     </row>
-    <row r="114" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A114" s="22" t="s">
         <v>19</v>
       </c>
@@ -5984,7 +5990,7 @@
       <c r="O114" s="22"/>
       <c r="P114" s="22"/>
     </row>
-    <row r="115" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A115" s="22" t="s">
         <v>19</v>
       </c>
@@ -6025,7 +6031,7 @@
       <c r="O115" s="22"/>
       <c r="P115" s="22"/>
     </row>
-    <row r="116" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A116" s="22"/>
       <c r="B116" s="23"/>
       <c r="C116" s="24"/>
@@ -6054,7 +6060,7 @@
       <c r="O116" s="22"/>
       <c r="P116" s="22"/>
     </row>
-    <row r="117" spans="1:16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A117" s="25" t="s">
         <v>163</v>
       </c>
@@ -6095,7 +6101,7 @@
       <c r="A118" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="B118" s="23" t="s">
+      <c r="B118" s="30" t="s">
         <v>314</v>
       </c>
       <c r="C118" s="24" t="s">
@@ -6137,7 +6143,7 @@
       </c>
       <c r="P118" s="22"/>
     </row>
-    <row r="119" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A119" s="22"/>
       <c r="B119" s="23"/>
       <c r="C119" s="24"/>
@@ -6166,7 +6172,7 @@
       <c r="O119" s="22"/>
       <c r="P119" s="22"/>
     </row>
-    <row r="120" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A120" s="25" t="s">
         <v>167</v>
       </c>
@@ -6252,7 +6258,7 @@
       </c>
       <c r="P121" s="27"/>
     </row>
-    <row r="122" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A122" s="22"/>
       <c r="B122" s="23"/>
       <c r="C122" s="24"/>
@@ -6281,7 +6287,7 @@
       <c r="O122" s="22"/>
       <c r="P122" s="22"/>
     </row>
-    <row r="123" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A123" s="25" t="s">
         <v>173</v>
       </c>
@@ -6364,7 +6370,7 @@
       </c>
       <c r="P124" s="22"/>
     </row>
-    <row r="125" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A125" s="22"/>
       <c r="B125" s="23"/>
       <c r="C125" s="24"/>
@@ -6393,7 +6399,7 @@
       <c r="O125" s="22"/>
       <c r="P125" s="22"/>
     </row>
-    <row r="126" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A126" s="25" t="s">
         <v>178</v>
       </c>
@@ -6426,7 +6432,7 @@
       <c r="O126" s="22"/>
       <c r="P126" s="22"/>
     </row>
-    <row r="127" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A127" s="22" t="s">
         <v>179</v>
       </c>
@@ -6467,7 +6473,7 @@
       <c r="O127" s="22"/>
       <c r="P127" s="22"/>
     </row>
-    <row r="128" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A128" s="22" t="s">
         <v>19</v>
       </c>
@@ -6508,7 +6514,7 @@
       <c r="O128" s="22"/>
       <c r="P128" s="22"/>
     </row>
-    <row r="129" spans="1:13" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:13" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A129" s="22" t="s">
         <v>19</v>
       </c>
@@ -6546,7 +6552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:13" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A130" s="22"/>
       <c r="B130" s="23"/>
       <c r="C130" s="24"/>
@@ -6572,7 +6578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:13" ht="12" hidden="1" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:13" ht="12" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A131" s="25" t="s">
         <v>184</v>
       </c>
@@ -6602,7 +6608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:13" s="19" customFormat="1" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:13" s="19" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A132" s="27" t="s">
         <v>185</v>
       </c>
@@ -6643,7 +6649,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="133" spans="1:13" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A133" s="22"/>
       <c r="B133" s="23"/>
       <c r="C133" s="24"/>
@@ -6669,7 +6675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:13" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A134" s="25" t="s">
         <v>189</v>
       </c>
@@ -6699,7 +6705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:13" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:13" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A135" s="22" t="s">
         <v>190</v>
       </c>
@@ -6737,7 +6743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:13" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:13" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A136" s="22" t="s">
         <v>19</v>
       </c>
@@ -6775,7 +6781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:13" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A137" s="22"/>
       <c r="B137" s="23"/>
       <c r="C137" s="24"/>
@@ -6801,7 +6807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:13" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A138" s="25" t="s">
         <v>194</v>
       </c>
@@ -6831,7 +6837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:13" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:13" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A139" s="22" t="s">
         <v>195</v>
       </c>
@@ -6869,7 +6875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:13" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:13" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A140" s="22" t="s">
         <v>19</v>
       </c>
@@ -6907,7 +6913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:13" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:13" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A141" s="22" t="s">
         <v>19</v>
       </c>
@@ -6945,7 +6951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:13" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:13" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A142" s="22" t="s">
         <v>19</v>
       </c>
@@ -6983,7 +6989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:13" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:13" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A143" s="22" t="s">
         <v>19</v>
       </c>
@@ -7021,7 +7027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:13" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:13" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A144" s="22" t="s">
         <v>19</v>
       </c>
@@ -7059,7 +7065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A145" s="22" t="s">
         <v>19</v>
       </c>
@@ -7100,7 +7106,7 @@
       <c r="O145" s="22"/>
       <c r="P145" s="22"/>
     </row>
-    <row r="146" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A146" s="22" t="s">
         <v>19</v>
       </c>
@@ -7141,7 +7147,7 @@
       <c r="O146" s="22"/>
       <c r="P146" s="22"/>
     </row>
-    <row r="147" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A147" s="22" t="s">
         <v>19</v>
       </c>
@@ -7182,7 +7188,7 @@
       <c r="O147" s="22"/>
       <c r="P147" s="22"/>
     </row>
-    <row r="148" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A148" s="22" t="s">
         <v>19</v>
       </c>
@@ -7223,7 +7229,7 @@
       <c r="O148" s="22"/>
       <c r="P148" s="22"/>
     </row>
-    <row r="149" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A149" s="22" t="s">
         <v>19</v>
       </c>
@@ -7264,7 +7270,7 @@
       <c r="O149" s="22"/>
       <c r="P149" s="22"/>
     </row>
-    <row r="150" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A150" s="22" t="s">
         <v>19</v>
       </c>
@@ -7305,7 +7311,7 @@
       <c r="O150" s="22"/>
       <c r="P150" s="22"/>
     </row>
-    <row r="151" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A151" s="22" t="s">
         <v>19</v>
       </c>
@@ -7346,7 +7352,7 @@
       <c r="O151" s="22"/>
       <c r="P151" s="22"/>
     </row>
-    <row r="152" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A152" s="22" t="s">
         <v>19</v>
       </c>
@@ -7387,7 +7393,7 @@
       <c r="O152" s="22"/>
       <c r="P152" s="22"/>
     </row>
-    <row r="153" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A153" s="22" t="s">
         <v>19</v>
       </c>
@@ -7428,7 +7434,7 @@
       <c r="O153" s="22"/>
       <c r="P153" s="22"/>
     </row>
-    <row r="154" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A154" s="22" t="s">
         <v>19</v>
       </c>
@@ -7469,7 +7475,7 @@
       <c r="O154" s="22"/>
       <c r="P154" s="22"/>
     </row>
-    <row r="155" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A155" s="22"/>
       <c r="B155" s="23"/>
       <c r="C155" s="24"/>
@@ -7498,7 +7504,7 @@
       <c r="O155" s="22"/>
       <c r="P155" s="22"/>
     </row>
-    <row r="156" spans="1:16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A156" s="25" t="s">
         <v>213</v>
       </c>
@@ -7581,7 +7587,7 @@
       </c>
       <c r="P157" s="22"/>
     </row>
-    <row r="158" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A158" s="22" t="s">
         <v>19</v>
       </c>
@@ -7622,7 +7628,7 @@
       <c r="O158" s="22"/>
       <c r="P158" s="22"/>
     </row>
-    <row r="159" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A159" s="22"/>
       <c r="B159" s="23"/>
       <c r="C159" s="24"/>
@@ -7651,7 +7657,7 @@
       <c r="O159" s="22"/>
       <c r="P159" s="22"/>
     </row>
-    <row r="160" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A160" s="25" t="s">
         <v>219</v>
       </c>
@@ -7734,7 +7740,7 @@
       </c>
       <c r="P161" s="22"/>
     </row>
-    <row r="162" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A162" s="22"/>
       <c r="B162" s="23"/>
       <c r="C162" s="24"/>
@@ -7763,7 +7769,7 @@
       <c r="O162" s="22"/>
       <c r="P162" s="22"/>
     </row>
-    <row r="163" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A163" s="25" t="s">
         <v>224</v>
       </c>
@@ -7796,7 +7802,7 @@
       <c r="O163" s="22"/>
       <c r="P163" s="22"/>
     </row>
-    <row r="164" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A164" s="22" t="s">
         <v>225</v>
       </c>
@@ -7837,7 +7843,7 @@
       <c r="O164" s="22"/>
       <c r="P164" s="22"/>
     </row>
-    <row r="165" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A165" s="22"/>
       <c r="B165" s="23"/>
       <c r="C165" s="24"/>
@@ -7866,7 +7872,7 @@
       <c r="O165" s="22"/>
       <c r="P165" s="22"/>
     </row>
-    <row r="166" spans="1:16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A166" s="25" t="s">
         <v>228</v>
       </c>
@@ -7899,7 +7905,7 @@
       <c r="O166" s="22"/>
       <c r="P166" s="22"/>
     </row>
-    <row r="167" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A167" s="22" t="s">
         <v>229</v>
       </c>
@@ -7940,7 +7946,7 @@
       <c r="O167" s="22"/>
       <c r="P167" s="22"/>
     </row>
-    <row r="168" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A168" s="22"/>
       <c r="B168" s="23"/>
       <c r="C168" s="24"/>
@@ -7969,7 +7975,7 @@
       <c r="O168" s="22"/>
       <c r="P168" s="22"/>
     </row>
-    <row r="169" spans="1:16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A169" s="25" t="s">
         <v>232</v>
       </c>
@@ -8002,7 +8008,7 @@
       <c r="O169" s="22"/>
       <c r="P169" s="22"/>
     </row>
-    <row r="170" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A170" s="27" t="s">
         <v>233</v>
       </c>
@@ -8046,7 +8052,7 @@
       <c r="O170" s="22"/>
       <c r="P170" s="22"/>
     </row>
-    <row r="171" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A171" s="22"/>
       <c r="B171" s="23"/>
       <c r="C171" s="24"/>
@@ -8075,7 +8081,7 @@
       <c r="O171" s="22"/>
       <c r="P171" s="22"/>
     </row>
-    <row r="172" spans="1:16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A172" s="25" t="s">
         <v>237</v>
       </c>
@@ -8108,7 +8114,7 @@
       <c r="O172" s="22"/>
       <c r="P172" s="22"/>
     </row>
-    <row r="173" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A173" s="22" t="s">
         <v>238</v>
       </c>
@@ -8149,7 +8155,7 @@
       <c r="O173" s="22"/>
       <c r="P173" s="22"/>
     </row>
-    <row r="174" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A174" s="22"/>
       <c r="B174" s="23"/>
       <c r="C174" s="24"/>
@@ -8178,7 +8184,7 @@
       <c r="O174" s="22"/>
       <c r="P174" s="22"/>
     </row>
-    <row r="175" spans="1:16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A175" s="25" t="s">
         <v>241</v>
       </c>
@@ -8261,7 +8267,7 @@
       </c>
       <c r="P176" s="22"/>
     </row>
-    <row r="177" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A177" s="22"/>
       <c r="B177" s="23"/>
       <c r="C177" s="24"/>
@@ -8290,7 +8296,7 @@
       <c r="O177" s="22"/>
       <c r="P177" s="22"/>
     </row>
-    <row r="178" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A178" s="25" t="s">
         <v>246</v>
       </c>
@@ -8323,7 +8329,7 @@
       <c r="O178" s="22"/>
       <c r="P178" s="22"/>
     </row>
-    <row r="179" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A179" s="22" t="s">
         <v>247</v>
       </c>
@@ -8364,7 +8370,7 @@
       <c r="O179" s="22"/>
       <c r="P179" s="22"/>
     </row>
-    <row r="180" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A180" s="22" t="s">
         <v>19</v>
       </c>
@@ -8405,7 +8411,7 @@
       <c r="O180" s="22"/>
       <c r="P180" s="22"/>
     </row>
-    <row r="181" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A181" s="22" t="s">
         <v>19</v>
       </c>
@@ -8446,7 +8452,7 @@
       <c r="O181" s="22"/>
       <c r="P181" s="22"/>
     </row>
-    <row r="182" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A182" s="22" t="s">
         <v>19</v>
       </c>
@@ -8487,7 +8493,7 @@
       <c r="O182" s="22"/>
       <c r="P182" s="22"/>
     </row>
-    <row r="183" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A183" s="22" t="s">
         <v>19</v>
       </c>
@@ -8528,7 +8534,7 @@
       <c r="O183" s="22"/>
       <c r="P183" s="22"/>
     </row>
-    <row r="184" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A184" s="22" t="s">
         <v>19</v>
       </c>
@@ -8569,7 +8575,7 @@
       <c r="O184" s="22"/>
       <c r="P184" s="22"/>
     </row>
-    <row r="185" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A185" s="22" t="s">
         <v>19</v>
       </c>
@@ -8610,7 +8616,7 @@
       <c r="O185" s="22"/>
       <c r="P185" s="22"/>
     </row>
-    <row r="186" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A186" s="22" t="s">
         <v>19</v>
       </c>
@@ -8651,7 +8657,7 @@
       <c r="O186" s="22"/>
       <c r="P186" s="22"/>
     </row>
-    <row r="187" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A187" s="22"/>
       <c r="B187" s="23"/>
       <c r="C187" s="24"/>
@@ -8680,7 +8686,7 @@
       <c r="O187" s="22"/>
       <c r="P187" s="22"/>
     </row>
-    <row r="188" spans="1:16" hidden="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A188" s="25" t="s">
         <v>256</v>
       </c>
@@ -8763,7 +8769,7 @@
       </c>
       <c r="P189" s="22"/>
     </row>
-    <row r="190" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A190" s="22"/>
       <c r="B190" s="23"/>
       <c r="C190" s="24"/>
@@ -8792,7 +8798,7 @@
       <c r="O190" s="22"/>
       <c r="P190" s="22"/>
     </row>
-    <row r="191" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A191" s="25" t="s">
         <v>261</v>
       </c>
@@ -8875,7 +8881,7 @@
       </c>
       <c r="P192" s="22"/>
     </row>
-    <row r="193" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A193" s="22" t="s">
         <v>19</v>
       </c>
@@ -8916,7 +8922,7 @@
       <c r="O193" s="22"/>
       <c r="P193" s="22"/>
     </row>
-    <row r="194" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A194" s="22" t="s">
         <v>19</v>
       </c>
@@ -8957,7 +8963,7 @@
       <c r="O194" s="22"/>
       <c r="P194" s="22"/>
     </row>
-    <row r="195" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A195" s="22" t="s">
         <v>19</v>
       </c>
@@ -8998,7 +9004,7 @@
       <c r="O195" s="22"/>
       <c r="P195" s="22"/>
     </row>
-    <row r="196" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A196" s="22" t="s">
         <v>19</v>
       </c>
@@ -9039,7 +9045,7 @@
       <c r="O196" s="22"/>
       <c r="P196" s="22"/>
     </row>
-    <row r="197" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A197" s="22" t="s">
         <v>19</v>
       </c>
@@ -9080,7 +9086,7 @@
       <c r="O197" s="22"/>
       <c r="P197" s="22"/>
     </row>
-    <row r="198" spans="1:16" hidden="1" outlineLevel="4" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:16" outlineLevel="4" x14ac:dyDescent="0.2">
       <c r="A198" s="22" t="s">
         <v>19</v>
       </c>
@@ -9121,7 +9127,7 @@
       <c r="O198" s="22"/>
       <c r="P198" s="22"/>
     </row>
-    <row r="199" spans="1:16" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:16" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A199" s="22"/>
       <c r="B199" s="23"/>
       <c r="C199" s="24"/>
@@ -9150,7 +9156,7 @@
       <c r="O199" s="22"/>
       <c r="P199" s="22"/>
     </row>
-    <row r="200" spans="1:16" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:16" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A200" s="25" t="s">
         <v>272</v>
       </c>
@@ -9427,13 +9433,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P201" xr:uid="{02726FE6-ECA2-4AE9-8D81-CEAB62872255}">
-    <filterColumn colId="13">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>